<commit_message>
Published state of ETDataset on 26 August 2016
</commit_message>
<xml_diff>
--- a/analyses/5_industry_analysis.xlsx
+++ b/analyses/5_industry_analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="835" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23460" tabRatio="835" firstSheet="5" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -250,7 +250,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1314" uniqueCount="696">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1301" uniqueCount="693">
   <si>
     <t>Changelog</t>
   </si>
@@ -1833,21 +1833,12 @@
     <t>Total non-energetic final consumption excl. refineries</t>
   </si>
   <si>
-    <t>Non-energetic consumption in Chemical industry sub-sector in ETM</t>
-  </si>
-  <si>
-    <t>Of which refineries</t>
-  </si>
-  <si>
     <t>Non-energetic consumption in Chemical industry sub-sector in EB (excl. refineries)</t>
   </si>
   <si>
     <t>Own use in refineries</t>
   </si>
   <si>
-    <t>Non-energetic final demand in referinies on energy balance</t>
-  </si>
-  <si>
     <t>Fuel Aggregation subsectors</t>
   </si>
   <si>
@@ -1879,9 +1870,6 @@
   </si>
   <si>
     <t>In this sheet the Energetic final demand in the Other industy sector is calculated from the own use and energetic consumption of the whole industry and the own use and energetic consumption in the Metal industry and Chemical industry sector. The Energetic final demand of the Metal industry sector is equal to the Energetic consumption, because the Own use is modelled outside the sector in the transformation part.</t>
-  </si>
-  <si>
-    <t>In this sheet the non-energetic final demand in the Other industy sub-sector from the whole industry and the Metal industry and Chemical industry sector.</t>
   </si>
   <si>
     <t>In this sheet the transformation that is not modelled in sectors is calculated to validate the sector modelling and to enable correction through coal loss calculations.</t>
@@ -2412,6 +2400,9 @@
   </si>
   <si>
     <t>Rob Terwel</t>
+  </si>
+  <si>
+    <t>In this sheet the non-energetic final demand in the Other industy sub-sector from the whole industry and the Metal industry and Chemical industry sector. The  non-energetic final demand for crude oil of the chemical industry is corrected for the oil products which refineries produce for the petrochemical industry; it is imported from the 'Non-energetic cons analysis' tab.</t>
   </si>
 </sst>
 </file>
@@ -3360,7 +3351,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1462">
+  <cellStyleXfs count="1470">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -4823,8 +4814,16 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="584">
+  <cellXfs count="588">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -5937,6 +5936,18 @@
     <xf numFmtId="3" fontId="22" fillId="15" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="41" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="16" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6010,7 +6021,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1462">
+  <cellStyles count="1470">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
@@ -6741,6 +6752,10 @@
     <cellStyle name="Followed Hyperlink" xfId="1457" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1459" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="1461" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1463" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1465" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1467" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="1469" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -7469,6 +7484,10 @@
     <cellStyle name="Hyperlink" xfId="1456" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1458" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1460" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1462" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1464" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1466" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1468" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
     <cellStyle name="Percent 2" xfId="772"/>
@@ -12478,67 +12497,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="7213600" cy="769441"/>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
-        <xdr:cNvSpPr txBox="1"/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10490200" y="609600"/>
-          <a:ext cx="7213600" cy="769441"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="lt1"/>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t">
-          <a:spAutoFit/>
-        </a:bodyPr>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100"/>
-            <a:t>Cell H17</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100" baseline="0"/>
-            <a:t> has been set to a hard-coded zero; when refineries are modelled better, it should be replaced with =SUM('Corrected energy balance step 2'![Cells[)), with Cells representing the EB transformation input for refineries as specified on row 33 of the EB, identical to that of the chemical_industry_analysis. In addition, it should be added to the demand of the node industry_final_demand_for_chemical_refineries_crude_oil_non_energetic</a:t>
-          </a:r>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -13405,7 +13363,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="D9" s="7"/>
     </row>
@@ -13600,7 +13558,7 @@
   <dimension ref="A1:Q28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -13681,13 +13639,13 @@
     </row>
     <row r="5" spans="1:17" ht="30" customHeight="1">
       <c r="A5" s="76"/>
-      <c r="B5" s="566" t="s">
+      <c r="B5" s="570" t="s">
         <v>475</v>
       </c>
-      <c r="C5" s="567"/>
-      <c r="D5" s="567"/>
-      <c r="E5" s="567"/>
-      <c r="F5" s="568"/>
+      <c r="C5" s="571"/>
+      <c r="D5" s="571"/>
+      <c r="E5" s="571"/>
+      <c r="F5" s="572"/>
       <c r="H5" s="76"/>
       <c r="I5" s="76"/>
       <c r="J5" s="76"/>
@@ -14183,11 +14141,11 @@
       <c r="E4" s="84"/>
     </row>
     <row r="5" spans="2:7" ht="60" customHeight="1">
-      <c r="B5" s="569" t="s">
+      <c r="B5" s="573" t="s">
         <v>479</v>
       </c>
-      <c r="C5" s="570"/>
-      <c r="D5" s="570"/>
+      <c r="C5" s="574"/>
+      <c r="D5" s="574"/>
       <c r="E5" s="84"/>
     </row>
     <row r="6" spans="2:7" ht="16" thickBot="1">
@@ -14257,7 +14215,7 @@
       </c>
       <c r="D12" s="482"/>
       <c r="E12" s="482" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="F12" s="484"/>
       <c r="G12" s="481">
@@ -14272,7 +14230,7 @@
       </c>
       <c r="D13" s="482"/>
       <c r="E13" s="482" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="F13" s="484"/>
       <c r="G13" s="481">
@@ -14287,7 +14245,7 @@
       </c>
       <c r="D14" s="482"/>
       <c r="E14" s="482" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="F14" s="484"/>
       <c r="G14" s="481">
@@ -14302,7 +14260,7 @@
       </c>
       <c r="D15" s="482"/>
       <c r="E15" s="482" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="F15" s="484"/>
       <c r="G15" s="481">
@@ -14366,12 +14324,12 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="571" t="s">
-        <v>530</v>
-      </c>
-      <c r="C5" s="572"/>
-      <c r="D5" s="572"/>
-      <c r="E5" s="573"/>
+      <c r="B5" s="575" t="s">
+        <v>527</v>
+      </c>
+      <c r="C5" s="576"/>
+      <c r="D5" s="576"/>
+      <c r="E5" s="577"/>
     </row>
     <row r="6" spans="2:7" ht="16" thickBot="1"/>
     <row r="7" spans="2:7">
@@ -14812,7 +14770,7 @@
   <dimension ref="B2:E25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -14838,12 +14796,12 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="2:5" ht="30" customHeight="1">
-      <c r="B5" s="571" t="s">
-        <v>531</v>
-      </c>
-      <c r="C5" s="572"/>
-      <c r="D5" s="572"/>
-      <c r="E5" s="573"/>
+      <c r="B5" s="575" t="s">
+        <v>528</v>
+      </c>
+      <c r="C5" s="576"/>
+      <c r="D5" s="576"/>
+      <c r="E5" s="577"/>
     </row>
     <row r="6" spans="2:5" ht="16" thickBot="1"/>
     <row r="7" spans="2:5">
@@ -14886,7 +14844,7 @@
         <v>428</v>
       </c>
       <c r="D11" s="390">
-        <f>'Non-energetic FD sectors'!D14</f>
+        <f>'Non-energetic FD sectors'!D13</f>
         <v>0</v>
       </c>
       <c r="E11" s="292">
@@ -14900,7 +14858,7 @@
         <v>82</v>
       </c>
       <c r="D12" s="390">
-        <f>'Non-energetic FD sectors'!D15</f>
+        <f>'Non-energetic FD sectors'!D14</f>
         <v>0</v>
       </c>
       <c r="E12" s="292">
@@ -14928,7 +14886,7 @@
         <v>428</v>
       </c>
       <c r="D15" s="390">
-        <f>'Non-energetic FD sectors'!G14</f>
+        <f>'Non-energetic FD sectors'!G13</f>
         <v>0</v>
       </c>
       <c r="E15" s="292">
@@ -14942,7 +14900,7 @@
         <v>82</v>
       </c>
       <c r="D16" s="390">
-        <f>'Non-energetic FD sectors'!G15</f>
+        <f>'Non-energetic FD sectors'!G14</f>
         <v>0</v>
       </c>
       <c r="E16" s="292">
@@ -14970,7 +14928,7 @@
         <v>428</v>
       </c>
       <c r="D19" s="390">
-        <f>'Non-energetic FD sectors'!H14</f>
+        <f>'Non-energetic FD sectors'!H13</f>
         <v>0</v>
       </c>
       <c r="E19" s="292">
@@ -14984,7 +14942,7 @@
         <v>82</v>
       </c>
       <c r="D20" s="390">
-        <f>'Non-energetic FD sectors'!H15</f>
+        <f>'Non-energetic FD sectors'!H14</f>
         <v>0</v>
       </c>
       <c r="E20" s="292">
@@ -15012,7 +14970,7 @@
         <v>428</v>
       </c>
       <c r="D23" s="390">
-        <f>'Non-energetic FD sectors'!I14</f>
+        <f>'Non-energetic FD sectors'!I13</f>
         <v>0</v>
       </c>
       <c r="E23" s="292">
@@ -15026,7 +14984,7 @@
         <v>82</v>
       </c>
       <c r="D24" s="390">
-        <f>'Non-energetic FD sectors'!I15</f>
+        <f>'Non-energetic FD sectors'!I14</f>
         <v>0</v>
       </c>
       <c r="E24" s="292">
@@ -15105,14 +15063,14 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:12" ht="60" customHeight="1">
-      <c r="B5" s="569" t="s">
-        <v>532</v>
-      </c>
-      <c r="C5" s="570"/>
-      <c r="D5" s="570"/>
-      <c r="E5" s="570"/>
-      <c r="F5" s="570"/>
-      <c r="G5" s="574"/>
+      <c r="B5" s="573" t="s">
+        <v>529</v>
+      </c>
+      <c r="C5" s="574"/>
+      <c r="D5" s="574"/>
+      <c r="E5" s="574"/>
+      <c r="F5" s="574"/>
+      <c r="G5" s="578"/>
     </row>
     <row r="6" spans="1:12" ht="16" thickBot="1"/>
     <row r="7" spans="1:12">
@@ -15234,7 +15192,7 @@
     <row r="12" spans="1:12">
       <c r="A12" s="160"/>
       <c r="B12" s="178" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="C12" s="208"/>
       <c r="D12" s="427">
@@ -15790,16 +15748,16 @@
   <sheetPr codeName="Sheet15" enableFormatConditionsCalculation="0">
     <tabColor theme="8" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="B2:L16"/>
+  <dimension ref="B2:L15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="76"/>
-    <col min="2" max="2" width="54" style="76" customWidth="1"/>
+    <col min="2" max="2" width="68" style="76" customWidth="1"/>
     <col min="3" max="3" width="2.83203125" style="202" customWidth="1"/>
     <col min="4" max="12" width="15.83203125" style="76" customWidth="1"/>
     <col min="13" max="16384" width="10.83203125" style="76"/>
@@ -15835,15 +15793,15 @@
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="2:12" ht="29" customHeight="1">
-      <c r="B5" s="569" t="s">
-        <v>533</v>
-      </c>
-      <c r="C5" s="570"/>
-      <c r="D5" s="570"/>
-      <c r="E5" s="570"/>
-      <c r="F5" s="570"/>
-      <c r="G5" s="574"/>
+    <row r="5" spans="2:12" ht="44" customHeight="1">
+      <c r="B5" s="573" t="s">
+        <v>692</v>
+      </c>
+      <c r="C5" s="574"/>
+      <c r="D5" s="574"/>
+      <c r="E5" s="574"/>
+      <c r="F5" s="574"/>
+      <c r="G5" s="578"/>
     </row>
     <row r="6" spans="2:12" ht="16" thickBot="1"/>
     <row r="7" spans="2:12">
@@ -15962,13 +15920,13 @@
     </row>
     <row r="12" spans="2:12">
       <c r="B12" s="178" t="s">
-        <v>521</v>
+        <v>485</v>
       </c>
       <c r="C12" s="197" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D12" s="427">
-        <f>'Non-energetic cons analysis'!D17</f>
+        <f>'Non-energetic cons analysis'!D14</f>
         <v>0</v>
       </c>
       <c r="E12" s="407" t="s">
@@ -15978,179 +15936,137 @@
         <v>264</v>
       </c>
       <c r="G12" s="427">
-        <f>'Non-energetic cons analysis'!G17</f>
+        <f>'Non-energetic cons analysis'!G14</f>
         <v>0</v>
       </c>
       <c r="H12" s="427">
-        <f>'Non-energetic cons analysis'!H17</f>
+        <f>'Non-energetic cons analysis'!H14</f>
         <v>0</v>
       </c>
       <c r="I12" s="427">
-        <f>'Non-energetic cons analysis'!I17</f>
+        <f>'Non-energetic cons analysis'!I14</f>
         <v>0</v>
       </c>
       <c r="J12" s="427">
-        <f>'Non-energetic cons analysis'!J17</f>
+        <f>'Non-energetic cons analysis'!J14</f>
         <v>0</v>
       </c>
       <c r="K12" s="427">
-        <f>'Non-energetic cons analysis'!K17</f>
+        <f>'Non-energetic cons analysis'!K14</f>
         <v>0</v>
       </c>
       <c r="L12" s="402">
-        <f>'Non-energetic cons analysis'!L17</f>
+        <f>'Non-energetic cons analysis'!L14</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:12">
       <c r="B13" s="178" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C13" s="197" t="s">
         <v>264</v>
       </c>
-      <c r="D13" s="427">
-        <f>'Non-energetic cons analysis'!D14</f>
-        <v>0</v>
-      </c>
-      <c r="E13" s="407" t="s">
-        <v>264</v>
-      </c>
-      <c r="F13" s="407" t="s">
-        <v>264</v>
-      </c>
-      <c r="G13" s="427">
-        <f>'Non-energetic cons analysis'!G14</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="427">
-        <f>'Non-energetic cons analysis'!H14</f>
-        <v>0</v>
-      </c>
-      <c r="I13" s="427">
-        <f>'Non-energetic cons analysis'!I14</f>
-        <v>0</v>
-      </c>
-      <c r="J13" s="427">
-        <f>'Non-energetic cons analysis'!J14</f>
-        <v>0</v>
-      </c>
-      <c r="K13" s="427">
-        <f>'Non-energetic cons analysis'!K14</f>
-        <v>0</v>
-      </c>
-      <c r="L13" s="402">
-        <f>'Non-energetic cons analysis'!L14</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12">
-      <c r="B14" s="179" t="s">
-        <v>486</v>
-      </c>
-      <c r="C14" s="200" t="s">
-        <v>264</v>
-      </c>
-      <c r="D14" s="500">
+      <c r="D13" s="469">
         <f>'Non-energetic cons analysis'!D16</f>
         <v>0</v>
       </c>
-      <c r="E14" s="439" t="str">
+      <c r="E13" s="407" t="str">
         <f>'Non-energetic cons analysis'!E16</f>
         <v>-</v>
       </c>
-      <c r="F14" s="439" t="str">
+      <c r="F13" s="407">
         <f>'Non-energetic cons analysis'!F16</f>
-        <v>-</v>
-      </c>
-      <c r="G14" s="428">
+        <v>0</v>
+      </c>
+      <c r="G13" s="407">
         <f>'Non-energetic cons analysis'!G16</f>
         <v>0</v>
       </c>
-      <c r="H14" s="428">
-        <f>'Non-energetic cons analysis'!H16</f>
-        <v>0</v>
-      </c>
-      <c r="I14" s="428">
+      <c r="H13" s="407">
+        <f>'Import from Chemical analysis'!G11</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="407">
         <f>'Non-energetic cons analysis'!I16</f>
         <v>0</v>
       </c>
-      <c r="J14" s="428">
+      <c r="J13" s="407">
         <f>'Non-energetic cons analysis'!J16</f>
         <v>0</v>
       </c>
-      <c r="K14" s="428">
+      <c r="K13" s="407">
         <f>'Non-energetic cons analysis'!K16</f>
         <v>0</v>
       </c>
-      <c r="L14" s="443">
+      <c r="L13" s="402">
         <f>'Non-energetic cons analysis'!L16</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:12">
-      <c r="B15" s="178" t="s">
+    <row r="14" spans="2:12">
+      <c r="B14" s="178" t="s">
         <v>328</v>
       </c>
-      <c r="C15" s="197"/>
-      <c r="D15" s="431">
-        <f>D11+D12-D13-D14</f>
-        <v>0</v>
-      </c>
-      <c r="E15" s="441" t="s">
+      <c r="C14" s="197"/>
+      <c r="D14" s="561">
+        <f>D11-D12-D13</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="562" t="s">
         <v>264</v>
       </c>
-      <c r="F15" s="441" t="s">
+      <c r="F14" s="562" t="s">
         <v>264</v>
       </c>
-      <c r="G15" s="431">
-        <f t="shared" ref="G15:L15" si="0">G11+G12-G13-G14</f>
-        <v>0</v>
-      </c>
-      <c r="H15" s="431">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I15" s="431">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J15" s="431">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K15" s="431">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="444">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" ht="16" thickBot="1">
-      <c r="B16" s="180"/>
-      <c r="C16" s="199"/>
-      <c r="D16" s="411"/>
-      <c r="E16" s="411"/>
-      <c r="F16" s="411"/>
-      <c r="G16" s="411"/>
-      <c r="H16" s="411"/>
-      <c r="I16" s="411"/>
-      <c r="J16" s="411"/>
-      <c r="K16" s="411"/>
-      <c r="L16" s="433"/>
+      <c r="G14" s="563">
+        <f>G11+G12-G13</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="563">
+        <f>'Non-energetic cons analysis'!H19</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="563">
+        <f>I11-I12-I13</f>
+        <v>0</v>
+      </c>
+      <c r="J14" s="563">
+        <f>J11-J12-J13</f>
+        <v>0</v>
+      </c>
+      <c r="K14" s="563">
+        <f>K11-K12-K13</f>
+        <v>0</v>
+      </c>
+      <c r="L14" s="560">
+        <f>L11-L12-L13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" ht="16" thickBot="1">
+      <c r="B15" s="180"/>
+      <c r="C15" s="199"/>
+      <c r="D15" s="411"/>
+      <c r="E15" s="411"/>
+      <c r="F15" s="411"/>
+      <c r="G15" s="411"/>
+      <c r="H15" s="411"/>
+      <c r="I15" s="411"/>
+      <c r="J15" s="411"/>
+      <c r="K15" s="411"/>
+      <c r="L15" s="433"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:G5"/>
   </mergeCells>
-  <conditionalFormatting sqref="H16:L16">
+  <conditionalFormatting sqref="H15:L15">
     <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D16:G16">
+  <conditionalFormatting sqref="D15:G15">
     <cfRule type="cellIs" dxfId="13" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -16158,7 +16074,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="D13:L13" emptyCellReference="1"/>
+    <ignoredError sqref="D12:L12" emptyCellReference="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -16218,14 +16134,14 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="2:12" ht="30" customHeight="1">
-      <c r="B5" s="569" t="s">
-        <v>534</v>
-      </c>
-      <c r="C5" s="570"/>
-      <c r="D5" s="570"/>
-      <c r="E5" s="570"/>
-      <c r="F5" s="570"/>
-      <c r="G5" s="574"/>
+      <c r="B5" s="573" t="s">
+        <v>530</v>
+      </c>
+      <c r="C5" s="574"/>
+      <c r="D5" s="574"/>
+      <c r="E5" s="574"/>
+      <c r="F5" s="574"/>
+      <c r="G5" s="578"/>
     </row>
     <row r="6" spans="2:12" ht="16" thickBot="1"/>
     <row r="7" spans="2:12">
@@ -16796,14 +16712,14 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="2:12" ht="29" customHeight="1">
-      <c r="B5" s="569" t="s">
-        <v>535</v>
-      </c>
-      <c r="C5" s="570"/>
-      <c r="D5" s="570"/>
-      <c r="E5" s="570"/>
-      <c r="F5" s="570"/>
-      <c r="G5" s="574"/>
+      <c r="B5" s="573" t="s">
+        <v>531</v>
+      </c>
+      <c r="C5" s="574"/>
+      <c r="D5" s="574"/>
+      <c r="E5" s="574"/>
+      <c r="F5" s="574"/>
+      <c r="G5" s="578"/>
     </row>
     <row r="6" spans="2:12" ht="16" thickBot="1"/>
     <row r="7" spans="2:12">
@@ -17290,14 +17206,14 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="2:12" ht="29" customHeight="1">
-      <c r="B5" s="569" t="s">
-        <v>536</v>
-      </c>
-      <c r="C5" s="570"/>
-      <c r="D5" s="570"/>
-      <c r="E5" s="570"/>
-      <c r="F5" s="570"/>
-      <c r="G5" s="574"/>
+      <c r="B5" s="573" t="s">
+        <v>532</v>
+      </c>
+      <c r="C5" s="574"/>
+      <c r="D5" s="574"/>
+      <c r="E5" s="574"/>
+      <c r="F5" s="574"/>
+      <c r="G5" s="578"/>
     </row>
     <row r="6" spans="2:12" ht="16" thickBot="1"/>
     <row r="7" spans="2:12">
@@ -17928,10 +17844,10 @@
   <sheetPr codeName="Sheet19" enableFormatConditionsCalculation="0">
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A2:L22"/>
+  <dimension ref="A2:L20"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -17974,14 +17890,14 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="2:12" ht="30" customHeight="1">
-      <c r="B5" s="569" t="s">
-        <v>537</v>
-      </c>
-      <c r="C5" s="570"/>
-      <c r="D5" s="570"/>
-      <c r="E5" s="570"/>
-      <c r="F5" s="570"/>
-      <c r="G5" s="574"/>
+      <c r="B5" s="573" t="s">
+        <v>533</v>
+      </c>
+      <c r="C5" s="574"/>
+      <c r="D5" s="574"/>
+      <c r="E5" s="574"/>
+      <c r="F5" s="574"/>
+      <c r="G5" s="578"/>
     </row>
     <row r="6" spans="2:12" ht="16" thickBot="1"/>
     <row r="7" spans="2:12">
@@ -18152,213 +18068,137 @@
       <c r="K15" s="497"/>
       <c r="L15" s="447"/>
     </row>
-    <row r="16" spans="2:12">
+    <row r="16" spans="2:12" ht="30">
       <c r="B16" s="496" t="s">
         <v>517</v>
       </c>
       <c r="C16" s="197"/>
       <c r="D16" s="435">
-        <f>'Import from Chemical analysis'!C11</f>
+        <f>SUM('Corrected energy balance step 2'!C89:N89,'Corrected energy balance step 2'!S89)</f>
         <v>0</v>
       </c>
       <c r="E16" s="492" t="s">
         <v>264</v>
       </c>
-      <c r="F16" s="492" t="s">
+      <c r="F16" s="492">
+        <f>SUM('Corrected energy balance step 2'!P89:R89)</f>
+        <v>0</v>
+      </c>
+      <c r="G16" s="435">
+        <f>SUM('Corrected energy balance step 2'!T89,'Corrected energy balance step 2'!AV89)</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="435">
+        <f>SUM('Corrected energy balance step 2'!U89:AQ89)</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="435">
+        <f>SUM('Corrected energy balance step 2'!AU89,'Corrected energy balance step 2'!AZ89)</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="435">
+        <f>'Corrected energy balance step 2'!BM89</f>
+        <v>0</v>
+      </c>
+      <c r="K16" s="427">
+        <f>'Corrected energy balance step 2'!BK83</f>
+        <v>0</v>
+      </c>
+      <c r="L16" s="437">
+        <f>SUM('Corrected energy balance step 2'!O89,'Corrected energy balance step 2'!U89,'Corrected energy balance step 2'!AT89,'Corrected energy balance step 2'!AW89:AY89,'Corrected energy balance step 2'!BA89,'Corrected energy balance step 2'!BB89:BK89)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="160"/>
+      <c r="B17" s="179"/>
+      <c r="C17" s="200"/>
+      <c r="D17" s="403"/>
+      <c r="E17" s="498"/>
+      <c r="F17" s="498"/>
+      <c r="G17" s="403"/>
+      <c r="H17" s="403"/>
+      <c r="I17" s="403"/>
+      <c r="J17" s="403"/>
+      <c r="K17" s="403"/>
+      <c r="L17" s="404"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="B18" s="178"/>
+      <c r="C18" s="197"/>
+      <c r="D18" s="405"/>
+      <c r="E18" s="499"/>
+      <c r="F18" s="499"/>
+      <c r="G18" s="405"/>
+      <c r="H18" s="405"/>
+      <c r="I18" s="405"/>
+      <c r="J18" s="405"/>
+      <c r="K18" s="405"/>
+      <c r="L18" s="406"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="B19" s="178" t="s">
+        <v>325</v>
+      </c>
+      <c r="C19" s="197"/>
+      <c r="D19" s="379">
+        <f>D11-D14-D16</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="461" t="s">
         <v>264</v>
       </c>
-      <c r="G16" s="435">
-        <f>'Import from Chemical analysis'!F11</f>
-        <v>0</v>
-      </c>
-      <c r="H16" s="435">
-        <f>'Import from Chemical analysis'!G11</f>
-        <v>0</v>
-      </c>
-      <c r="I16" s="435">
-        <f>'Import from Chemical analysis'!H11</f>
-        <v>0</v>
-      </c>
-      <c r="J16" s="435">
-        <f>'Import from Chemical analysis'!I11</f>
-        <v>0</v>
-      </c>
-      <c r="K16" s="435">
-        <f>'Import from Chemical analysis'!J11</f>
-        <v>0</v>
-      </c>
-      <c r="L16" s="437">
-        <f>'Import from Chemical analysis'!K11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12">
-      <c r="B17" s="496" t="s">
-        <v>518</v>
-      </c>
-      <c r="C17" s="197"/>
-      <c r="D17" s="435">
-        <v>0</v>
-      </c>
-      <c r="E17" s="492" t="s">
+      <c r="F19" s="461" t="s">
         <v>264</v>
       </c>
-      <c r="F17" s="492" t="s">
-        <v>264</v>
-      </c>
-      <c r="G17" s="435">
-        <v>0</v>
-      </c>
-      <c r="H17" s="435">
-        <v>0</v>
-      </c>
-      <c r="I17" s="435">
-        <v>0</v>
-      </c>
-      <c r="J17" s="435">
-        <v>0</v>
-      </c>
-      <c r="K17" s="435">
-        <v>0</v>
-      </c>
-      <c r="L17" s="437">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="30">
-      <c r="B18" s="496" t="s">
-        <v>519</v>
-      </c>
-      <c r="C18" s="197" t="s">
-        <v>264</v>
-      </c>
-      <c r="D18" s="435">
-        <f>D16-D17</f>
-        <v>0</v>
-      </c>
-      <c r="E18" s="492" t="s">
-        <v>264</v>
-      </c>
-      <c r="F18" s="492" t="s">
-        <v>264</v>
-      </c>
-      <c r="G18" s="435">
-        <f t="shared" ref="G18:L18" si="0">G16-G17</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="435">
+      <c r="G19" s="379">
+        <f t="shared" ref="G19:L19" si="0">G11-G14-G16</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="379">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I18" s="435">
+      <c r="I19" s="379">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J18" s="435">
+      <c r="J19" s="379">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K18" s="435">
+      <c r="K19" s="379">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L18" s="437">
+      <c r="L19" s="380">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:12">
-      <c r="A19" s="160"/>
-      <c r="B19" s="179"/>
-      <c r="C19" s="200" t="s">
-        <v>264</v>
-      </c>
-      <c r="D19" s="403"/>
-      <c r="E19" s="498"/>
-      <c r="F19" s="498"/>
-      <c r="G19" s="403"/>
-      <c r="H19" s="403"/>
-      <c r="I19" s="403"/>
-      <c r="J19" s="403"/>
-      <c r="K19" s="403"/>
-      <c r="L19" s="404"/>
-    </row>
-    <row r="20" spans="1:12">
-      <c r="B20" s="178"/>
-      <c r="C20" s="197"/>
-      <c r="D20" s="405"/>
-      <c r="E20" s="499"/>
-      <c r="F20" s="499"/>
-      <c r="G20" s="405"/>
-      <c r="H20" s="405"/>
-      <c r="I20" s="405"/>
-      <c r="J20" s="405"/>
-      <c r="K20" s="405"/>
-      <c r="L20" s="406"/>
-    </row>
-    <row r="21" spans="1:12">
-      <c r="B21" s="178" t="s">
-        <v>325</v>
-      </c>
-      <c r="C21" s="197"/>
-      <c r="D21" s="379">
-        <f>D11-D14-D18</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="461" t="s">
-        <v>264</v>
-      </c>
-      <c r="F21" s="461" t="s">
-        <v>264</v>
-      </c>
-      <c r="G21" s="379">
-        <f t="shared" ref="G21:L21" si="1">G11-G14-G18</f>
-        <v>0</v>
-      </c>
-      <c r="H21" s="379">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I21" s="379">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J21" s="379">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K21" s="379">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L21" s="380">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="16" thickBot="1">
-      <c r="B22" s="180"/>
-      <c r="C22" s="199"/>
-      <c r="D22" s="411"/>
-      <c r="E22" s="446"/>
-      <c r="F22" s="446"/>
-      <c r="G22" s="411"/>
-      <c r="H22" s="411"/>
-      <c r="I22" s="411"/>
-      <c r="J22" s="411"/>
-      <c r="K22" s="411"/>
-      <c r="L22" s="412"/>
+    <row r="20" spans="1:12" ht="16" thickBot="1">
+      <c r="B20" s="180"/>
+      <c r="C20" s="199"/>
+      <c r="D20" s="411"/>
+      <c r="E20" s="446"/>
+      <c r="F20" s="446"/>
+      <c r="G20" s="411"/>
+      <c r="H20" s="411"/>
+      <c r="I20" s="411"/>
+      <c r="J20" s="411"/>
+      <c r="K20" s="411"/>
+      <c r="L20" s="412"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:G5"/>
   </mergeCells>
-  <conditionalFormatting sqref="H22:L22">
+  <conditionalFormatting sqref="H20:L20">
     <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:G22">
+  <conditionalFormatting sqref="D20:G20">
     <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -18366,9 +18206,8 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="D19:L20 E21:F21 D16:L16" emptyCellReference="1"/>
+    <ignoredError sqref="D17:L18 E19:F19" emptyCellReference="1"/>
   </ignoredErrors>
-  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -18995,7 +18834,7 @@
         <v>42571</v>
       </c>
       <c r="C58" s="158" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="D58" s="159">
         <v>1.5</v>
@@ -19006,7 +18845,7 @@
         <v>42576</v>
       </c>
       <c r="C59" s="157" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="D59" s="159">
         <v>1.51</v>
@@ -19078,11 +18917,11 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="2:8" ht="45" customHeight="1">
-      <c r="B5" s="575" t="s">
+      <c r="B5" s="579" t="s">
         <v>363</v>
       </c>
-      <c r="C5" s="576"/>
-      <c r="D5" s="577"/>
+      <c r="C5" s="580"/>
+      <c r="D5" s="581"/>
       <c r="E5" s="167"/>
     </row>
     <row r="6" spans="2:8" ht="16" thickBot="1"/>
@@ -19309,15 +19148,15 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="2:13" ht="90" customHeight="1">
-      <c r="B5" s="578" t="s">
+      <c r="B5" s="582" t="s">
         <v>513</v>
       </c>
-      <c r="C5" s="579"/>
-      <c r="D5" s="579"/>
-      <c r="E5" s="579"/>
-      <c r="F5" s="579"/>
-      <c r="G5" s="579"/>
-      <c r="H5" s="580"/>
+      <c r="C5" s="583"/>
+      <c r="D5" s="583"/>
+      <c r="E5" s="583"/>
+      <c r="F5" s="583"/>
+      <c r="G5" s="583"/>
+      <c r="H5" s="584"/>
     </row>
     <row r="6" spans="2:13" ht="16" thickBot="1"/>
     <row r="7" spans="2:13">
@@ -19923,7 +19762,7 @@
   <sheetData>
     <row r="2" spans="2:13" ht="20">
       <c r="B2" s="75" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="C2" s="75"/>
       <c r="D2" s="75"/>
@@ -19955,15 +19794,15 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="2:13" ht="55" customHeight="1">
-      <c r="B5" s="581" t="s">
-        <v>692</v>
-      </c>
-      <c r="C5" s="582"/>
-      <c r="D5" s="582"/>
-      <c r="E5" s="582"/>
-      <c r="F5" s="582"/>
-      <c r="G5" s="582"/>
-      <c r="H5" s="583"/>
+      <c r="B5" s="585" t="s">
+        <v>688</v>
+      </c>
+      <c r="C5" s="586"/>
+      <c r="D5" s="586"/>
+      <c r="E5" s="586"/>
+      <c r="F5" s="586"/>
+      <c r="G5" s="586"/>
+      <c r="H5" s="587"/>
     </row>
     <row r="6" spans="2:13" ht="16" thickBot="1"/>
     <row r="7" spans="2:13">
@@ -20735,7 +20574,7 @@
   <sheetData>
     <row r="2" spans="1:13" ht="20">
       <c r="B2" s="75" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C2" s="75"/>
       <c r="D2" s="181"/>
@@ -20767,15 +20606,15 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:13" ht="60" customHeight="1">
-      <c r="B5" s="581" t="s">
-        <v>694</v>
-      </c>
-      <c r="C5" s="582"/>
-      <c r="D5" s="582"/>
-      <c r="E5" s="582"/>
-      <c r="F5" s="582"/>
-      <c r="G5" s="582"/>
-      <c r="H5" s="583"/>
+      <c r="B5" s="585" t="s">
+        <v>690</v>
+      </c>
+      <c r="C5" s="586"/>
+      <c r="D5" s="586"/>
+      <c r="E5" s="586"/>
+      <c r="F5" s="586"/>
+      <c r="G5" s="586"/>
+      <c r="H5" s="587"/>
     </row>
     <row r="6" spans="1:13" ht="16" thickBot="1"/>
     <row r="7" spans="1:13">
@@ -20858,7 +20697,7 @@
     <row r="11" spans="1:13">
       <c r="A11" s="160"/>
       <c r="B11" s="531" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C11" s="532"/>
       <c r="D11" s="208"/>
@@ -20902,7 +20741,7 @@
     <row r="12" spans="1:13">
       <c r="A12" s="160"/>
       <c r="B12" s="533" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="C12" s="534"/>
       <c r="D12" s="200" t="s">
@@ -20948,7 +20787,7 @@
     <row r="13" spans="1:13">
       <c r="A13" s="160"/>
       <c r="B13" s="531" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="C13" s="532"/>
       <c r="D13" s="197"/>
@@ -21018,7 +20857,7 @@
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="541" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="C16" s="542"/>
       <c r="D16" s="197"/>
@@ -21535,7 +21374,7 @@
   <sheetData>
     <row r="2" spans="1:13" ht="20">
       <c r="B2" s="75" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
       <c r="C2" s="75"/>
       <c r="D2" s="181"/>
@@ -21567,15 +21406,15 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:13" ht="39" customHeight="1">
-      <c r="B5" s="569" t="s">
-        <v>693</v>
-      </c>
-      <c r="C5" s="570"/>
-      <c r="D5" s="570"/>
-      <c r="E5" s="570"/>
-      <c r="F5" s="570"/>
-      <c r="G5" s="570"/>
-      <c r="H5" s="574"/>
+      <c r="B5" s="573" t="s">
+        <v>689</v>
+      </c>
+      <c r="C5" s="574"/>
+      <c r="D5" s="574"/>
+      <c r="E5" s="574"/>
+      <c r="F5" s="574"/>
+      <c r="G5" s="574"/>
+      <c r="H5" s="578"/>
     </row>
     <row r="6" spans="1:13" ht="16" thickBot="1"/>
     <row r="7" spans="1:13">
@@ -21657,7 +21496,7 @@
     <row r="11" spans="1:13">
       <c r="A11" s="160"/>
       <c r="B11" s="531" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="C11" s="532"/>
       <c r="D11" s="208"/>
@@ -21701,7 +21540,7 @@
     <row r="12" spans="1:13">
       <c r="A12" s="160"/>
       <c r="B12" s="533" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="C12" s="534"/>
       <c r="D12" s="200" t="s">
@@ -21747,7 +21586,7 @@
     <row r="13" spans="1:13">
       <c r="A13" s="160"/>
       <c r="B13" s="531" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="C13" s="532"/>
       <c r="D13" s="197"/>
@@ -21804,7 +21643,7 @@
     <row r="15" spans="1:13">
       <c r="A15" s="160"/>
       <c r="B15" s="556" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="C15" s="537"/>
       <c r="D15" s="538"/>
@@ -22262,12 +22101,12 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="571" t="s">
+      <c r="B5" s="575" t="s">
         <v>484</v>
       </c>
-      <c r="C5" s="572"/>
-      <c r="D5" s="572"/>
-      <c r="E5" s="573"/>
+      <c r="C5" s="576"/>
+      <c r="D5" s="576"/>
+      <c r="E5" s="577"/>
     </row>
     <row r="6" spans="2:7" ht="16" thickBot="1"/>
     <row r="7" spans="2:7">
@@ -23500,12 +23339,12 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="2:7">
-      <c r="B5" s="571" t="s">
+      <c r="B5" s="575" t="s">
         <v>484</v>
       </c>
-      <c r="C5" s="572"/>
-      <c r="D5" s="572"/>
-      <c r="E5" s="573"/>
+      <c r="C5" s="576"/>
+      <c r="D5" s="576"/>
+      <c r="E5" s="577"/>
     </row>
     <row r="6" spans="2:7" ht="16" thickBot="1"/>
     <row r="7" spans="2:7">
@@ -25021,23 +24860,23 @@
     </row>
     <row r="16" spans="2:3" ht="28" customHeight="1">
       <c r="B16" s="119" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C16" s="73" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="28" customHeight="1">
       <c r="B17" s="119" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C17" s="73" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="18" spans="2:3" ht="28" customHeight="1">
       <c r="B18" s="118" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="C18" s="73" t="s">
         <v>315</v>
@@ -25045,7 +24884,7 @@
     </row>
     <row r="19" spans="2:3" ht="28" customHeight="1">
       <c r="B19" s="118" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="C19" s="73" t="s">
         <v>316</v>
@@ -25093,50 +24932,50 @@
     </row>
     <row r="25" spans="2:3" ht="28" customHeight="1">
       <c r="B25" s="117" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="C25" s="125" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="28" customHeight="1">
       <c r="B26" s="117" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="C26" s="125" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="28" customHeight="1">
       <c r="B27" s="118" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="C27" s="73" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="28" customHeight="1">
       <c r="B28" s="118" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="C28" s="73" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="28" customHeight="1">
       <c r="B29" s="119" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="C29" s="73" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="28" customHeight="1">
       <c r="B30" s="119" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="C30" s="73" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="28" customHeight="1">
@@ -25144,7 +24983,7 @@
         <v>367</v>
       </c>
       <c r="C31" s="73" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="28" customHeight="1">
@@ -25152,7 +24991,7 @@
         <v>371</v>
       </c>
       <c r="C32" s="126" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="28" customHeight="1">
@@ -25160,7 +24999,7 @@
         <v>369</v>
       </c>
       <c r="C33" s="126" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="28" customHeight="1">
@@ -25168,7 +25007,7 @@
         <v>368</v>
       </c>
       <c r="C34" s="73" t="s">
-        <v>669</v>
+        <v>665</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="28" customHeight="1">
@@ -25176,7 +25015,7 @@
         <v>372</v>
       </c>
       <c r="C35" s="126" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="28" customHeight="1">
@@ -25184,7 +25023,7 @@
         <v>370</v>
       </c>
       <c r="C36" s="126" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="28" customHeight="1">
@@ -25192,7 +25031,7 @@
         <v>366</v>
       </c>
       <c r="C37" s="73" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="28" customHeight="1">
@@ -25200,7 +25039,7 @@
         <v>447</v>
       </c>
       <c r="C38" s="73" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="28" customHeight="1">
@@ -25208,7 +25047,7 @@
         <v>449</v>
       </c>
       <c r="C39" s="73" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="28" customHeight="1">
@@ -25216,7 +25055,7 @@
         <v>451</v>
       </c>
       <c r="C40" s="73" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="28" customHeight="1">
@@ -25224,7 +25063,7 @@
         <v>453</v>
       </c>
       <c r="C41" s="73" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="28" customHeight="1">
@@ -25232,7 +25071,7 @@
         <v>455</v>
       </c>
       <c r="C42" s="73" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="28" customHeight="1">
@@ -25253,7 +25092,7 @@
     </row>
     <row r="45" spans="2:3" ht="28" customHeight="1">
       <c r="B45" s="120" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="C45" s="73" t="s">
         <v>304</v>
@@ -25261,7 +25100,7 @@
     </row>
     <row r="46" spans="2:3" ht="28" customHeight="1">
       <c r="B46" s="120" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="C46" s="73" t="s">
         <v>305</v>
@@ -25269,7 +25108,7 @@
     </row>
     <row r="47" spans="2:3" ht="28" customHeight="1">
       <c r="B47" s="120" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="C47" s="126" t="s">
         <v>306</v>
@@ -25277,7 +25116,7 @@
     </row>
     <row r="48" spans="2:3" ht="28" customHeight="1">
       <c r="B48" s="120" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="C48" s="126" t="s">
         <v>302</v>
@@ -25285,7 +25124,7 @@
     </row>
     <row r="49" spans="2:3" ht="28" customHeight="1">
       <c r="B49" s="120" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="C49" s="126" t="s">
         <v>307</v>
@@ -25293,7 +25132,7 @@
     </row>
     <row r="50" spans="2:3" ht="28" customHeight="1">
       <c r="B50" s="120" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="C50" s="73" t="s">
         <v>303</v>
@@ -25301,7 +25140,7 @@
     </row>
     <row r="51" spans="2:3" ht="28" customHeight="1">
       <c r="B51" s="120" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="C51" s="73" t="s">
         <v>448</v>
@@ -25309,7 +25148,7 @@
     </row>
     <row r="52" spans="2:3" ht="28" customHeight="1">
       <c r="B52" s="120" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="C52" s="73" t="s">
         <v>450</v>
@@ -25317,7 +25156,7 @@
     </row>
     <row r="53" spans="2:3" ht="28" customHeight="1">
       <c r="B53" s="120" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="C53" s="73" t="s">
         <v>452</v>
@@ -25325,7 +25164,7 @@
     </row>
     <row r="54" spans="2:3" ht="28" customHeight="1">
       <c r="B54" s="120" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="C54" s="73" t="s">
         <v>454</v>
@@ -25871,7 +25710,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -25884,7 +25723,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="B3" s="452">
         <f>'Shares energetic FD subsectors'!E11</f>
@@ -25893,7 +25732,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="B4" s="452">
         <f>'Shares energetic FD subsectors'!E12</f>
@@ -25902,7 +25741,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B5" s="452">
         <f>'Shares energetic FD subsectors'!E13</f>
@@ -25911,7 +25750,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="B6" s="452">
         <f>'Shares energetic FD subsectors'!E14</f>
@@ -25920,7 +25759,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="B7" s="452">
         <f>'Shares energetic FD subsectors'!E15</f>
@@ -25929,7 +25768,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="B8" s="452">
         <f>'Shares energetic FD subsectors'!E16</f>
@@ -25938,7 +25777,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="B9" s="452">
         <f>'Shares energetic FD subsectors'!E17</f>
@@ -25947,7 +25786,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="B10" s="452">
         <f>'Shares energetic FD subsectors'!E18</f>
@@ -25956,7 +25795,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="B11" s="452">
         <f>'Shares energetic FD subsectors'!E19</f>
@@ -25965,7 +25804,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="B12" s="452">
         <f>'Shares energetic FD subsectors'!E20</f>
@@ -26114,7 +25953,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -26127,7 +25966,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="B3" s="452">
         <f>'Shares energetic FD subsectors'!E23</f>
@@ -26136,7 +25975,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="B4" s="452">
         <f>'Shares energetic FD subsectors'!E24</f>
@@ -26145,7 +25984,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="B5" s="452">
         <f>'Shares energetic FD subsectors'!E25</f>
@@ -26154,7 +25993,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B6" s="452">
         <f>'Shares energetic FD subsectors'!E26</f>
@@ -26163,7 +26002,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="B7" s="452">
         <f>'Shares energetic FD subsectors'!E27</f>
@@ -26172,7 +26011,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="B8" s="452">
         <f>'Shares energetic FD subsectors'!E28</f>
@@ -26181,7 +26020,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B9" s="452">
         <f>'Shares energetic FD subsectors'!E29</f>
@@ -26190,7 +26029,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B10" s="452">
         <f>'Shares energetic FD subsectors'!E30</f>
@@ -26199,7 +26038,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="B11" s="452">
         <f>'Shares energetic FD subsectors'!E31</f>
@@ -26208,7 +26047,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="B12" s="452">
         <f>'Shares energetic FD subsectors'!E32</f>
@@ -26241,7 +26080,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -26254,7 +26093,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="B3" s="452">
         <f>'Shares energetic FD subsectors'!E35</f>
@@ -26263,7 +26102,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="B4" s="452">
         <f>'Shares energetic FD subsectors'!E36</f>
@@ -26272,7 +26111,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="B5" s="452">
         <f>'Shares energetic FD subsectors'!E37</f>
@@ -26281,7 +26120,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="B6" s="452">
         <f>'Shares energetic FD subsectors'!E38</f>
@@ -26290,7 +26129,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="B7" s="452">
         <f>'Shares energetic FD subsectors'!E39</f>
@@ -26299,7 +26138,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="B8" s="452">
         <f>'Shares energetic FD subsectors'!E40</f>
@@ -26308,7 +26147,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="B9" s="452">
         <f>'Shares energetic FD subsectors'!E41</f>
@@ -26317,7 +26156,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="B10" s="452">
         <f>'Shares energetic FD subsectors'!E42</f>
@@ -26326,7 +26165,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="B11" s="452">
         <f>'Shares energetic FD subsectors'!E43</f>
@@ -26335,7 +26174,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="B12" s="452">
         <f>'Shares energetic FD subsectors'!E44</f>
@@ -26368,7 +26207,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -26381,7 +26220,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="B3" s="452">
         <f>'Shares energetic FD subsectors'!E47</f>
@@ -26390,7 +26229,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="B4" s="452">
         <f>'Shares energetic FD subsectors'!E48</f>
@@ -26399,7 +26238,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="B5" s="452">
         <f>'Shares energetic FD subsectors'!E49</f>
@@ -26408,7 +26247,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="B6" s="452">
         <f>'Shares energetic FD subsectors'!E50</f>
@@ -26417,7 +26256,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="B7" s="452">
         <f>'Shares energetic FD subsectors'!E51</f>
@@ -26426,7 +26265,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="B8" s="452">
         <f>'Shares energetic FD subsectors'!E52</f>
@@ -26435,7 +26274,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="B9" s="452">
         <f>'Shares energetic FD subsectors'!E53</f>
@@ -26444,7 +26283,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="B10" s="452">
         <f>'Shares energetic FD subsectors'!E54</f>
@@ -26453,7 +26292,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="B11" s="452">
         <f>'Shares energetic FD subsectors'!E55</f>
@@ -26462,7 +26301,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="B12" s="452">
         <f>'Shares energetic FD subsectors'!E56</f>
@@ -26495,7 +26334,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -26508,7 +26347,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="B3" s="452">
         <f>'Shares energetic FD subsectors'!E59</f>
@@ -26517,7 +26356,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="B4" s="452">
         <f>'Shares energetic FD subsectors'!E60</f>
@@ -26526,7 +26365,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="B5" s="452">
         <f>'Shares energetic FD subsectors'!E61</f>
@@ -26535,7 +26374,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="B6" s="452">
         <f>'Shares energetic FD subsectors'!E62</f>
@@ -26544,7 +26383,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="B7" s="452">
         <f>'Shares energetic FD subsectors'!E63</f>
@@ -26553,7 +26392,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="B8" s="452">
         <f>'Shares energetic FD subsectors'!E64</f>
@@ -26562,7 +26401,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>589</v>
+        <v>585</v>
       </c>
       <c r="B9" s="452">
         <f>'Shares energetic FD subsectors'!E65</f>
@@ -26571,7 +26410,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="B10" s="452">
         <f>'Shares energetic FD subsectors'!E66</f>
@@ -26580,7 +26419,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
       <c r="B11" s="452">
         <f>'Shares energetic FD subsectors'!E67</f>
@@ -26589,7 +26428,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
       <c r="B12" s="452">
         <f>'Shares energetic FD subsectors'!E68</f>
@@ -26622,7 +26461,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -26635,7 +26474,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
       <c r="B3" s="452">
         <f>'Shares energetic FD subsectors'!E71</f>
@@ -26644,7 +26483,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
       <c r="B4" s="452">
         <f>'Shares energetic FD subsectors'!E72</f>
@@ -26653,7 +26492,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="B5" s="452">
         <f>'Shares energetic FD subsectors'!E73</f>
@@ -26662,7 +26501,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="B6" s="452">
         <f>'Shares energetic FD subsectors'!E74</f>
@@ -26671,7 +26510,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="B7" s="452">
         <f>'Shares energetic FD subsectors'!E75</f>
@@ -26680,7 +26519,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="B8" s="452">
         <f>'Shares energetic FD subsectors'!E76</f>
@@ -26689,7 +26528,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>600</v>
+        <v>596</v>
       </c>
       <c r="B9" s="452">
         <f>'Shares energetic FD subsectors'!E77</f>
@@ -26698,7 +26537,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="B10" s="452">
         <f>'Shares energetic FD subsectors'!E78</f>
@@ -26707,7 +26546,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="B11" s="452">
         <f>'Shares energetic FD subsectors'!E79</f>
@@ -26716,7 +26555,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="B12" s="452">
         <f>'Shares energetic FD subsectors'!E80</f>
@@ -26749,7 +26588,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -26762,7 +26601,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="B3" s="452">
         <f>'Shares non-e FD subsectors'!E11</f>
@@ -26771,7 +26610,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>622</v>
+        <v>618</v>
       </c>
       <c r="B4" s="452">
         <f>'Shares non-e FD subsectors'!E12</f>
@@ -26780,7 +26619,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>623</v>
+        <v>619</v>
       </c>
       <c r="B5" s="452">
         <f>'Shares non-e FD subsectors'!E13</f>
@@ -26789,7 +26628,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="B6" s="452">
         <f>'Shares non-e FD subsectors'!E14</f>
@@ -26798,7 +26637,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>625</v>
+        <v>621</v>
       </c>
       <c r="B7" s="452">
         <f>'Shares non-e FD subsectors'!E15</f>
@@ -26807,7 +26646,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="B8" s="452">
         <f>'Shares non-e FD subsectors'!E16</f>
@@ -26816,7 +26655,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="B9" s="452">
         <f>'Shares non-e FD subsectors'!E17</f>
@@ -26825,7 +26664,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="B10" s="452">
         <f>'Shares non-e FD subsectors'!E18</f>
@@ -26834,7 +26673,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="B11" s="452">
         <f>'Shares non-e FD subsectors'!E19</f>
@@ -26843,7 +26682,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="B12" s="452">
         <f>'Shares non-e FD subsectors'!E20</f>
@@ -26876,7 +26715,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -26889,7 +26728,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="B3" s="452">
         <f>'Shares non-e FD subsectors'!E23</f>
@@ -26898,7 +26737,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="B4" s="452">
         <f>'Shares non-e FD subsectors'!E24</f>
@@ -26907,7 +26746,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="B5" s="452">
         <f>'Shares non-e FD subsectors'!E25</f>
@@ -26916,7 +26755,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="B6" s="452">
         <f>'Shares non-e FD subsectors'!E26</f>
@@ -26925,7 +26764,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="B7" s="452">
         <f>'Shares non-e FD subsectors'!E27</f>
@@ -26934,7 +26773,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="B8" s="452">
         <f>'Shares non-e FD subsectors'!E28</f>
@@ -26943,7 +26782,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="B9" s="452">
         <f>'Shares non-e FD subsectors'!E29</f>
@@ -26952,7 +26791,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>619</v>
+        <v>615</v>
       </c>
       <c r="B10" s="452">
         <f>'Shares non-e FD subsectors'!E30</f>
@@ -26961,7 +26800,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>620</v>
+        <v>616</v>
       </c>
       <c r="B11" s="452">
         <f>'Shares non-e FD subsectors'!E31</f>
@@ -26970,7 +26809,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>621</v>
+        <v>617</v>
       </c>
       <c r="B12" s="452">
         <f>'Shares non-e FD subsectors'!E32</f>
@@ -27003,7 +26842,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -27016,7 +26855,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="B3" s="452">
         <f>'Shares non-e FD subsectors'!E35</f>
@@ -27025,7 +26864,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="B4" s="452">
         <f>'Shares non-e FD subsectors'!E36</f>
@@ -27034,7 +26873,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="B5" s="452">
         <f>'Shares non-e FD subsectors'!E37</f>
@@ -27043,7 +26882,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="B6" s="452">
         <f>'Shares non-e FD subsectors'!E38</f>
@@ -27052,7 +26891,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="B7" s="452">
         <f>'Shares non-e FD subsectors'!E39</f>
@@ -27061,7 +26900,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="B8" s="452">
         <f>'Shares non-e FD subsectors'!E40</f>
@@ -27070,7 +26909,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="B9" s="452">
         <f>'Shares non-e FD subsectors'!E41</f>
@@ -27079,7 +26918,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="B10" s="452">
         <f>'Shares non-e FD subsectors'!E42</f>
@@ -27088,7 +26927,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="B11" s="452">
         <f>'Shares non-e FD subsectors'!E43</f>
@@ -27097,7 +26936,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="B12" s="452">
         <f>'Shares non-e FD subsectors'!E44</f>
@@ -27130,7 +26969,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -27143,7 +26982,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="B3" s="452">
         <f>'Shares non-e FD subsectors'!E47</f>
@@ -27152,7 +26991,7 @@
     </row>
     <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="B4" s="452">
         <f>'Shares non-e FD subsectors'!E48</f>
@@ -27161,7 +27000,7 @@
     </row>
     <row r="5" spans="1:2">
       <c r="A5" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="B5" s="452">
         <f>'Shares non-e FD subsectors'!E49</f>
@@ -27170,7 +27009,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="B6" s="452">
         <f>'Shares non-e FD subsectors'!E50</f>
@@ -27179,7 +27018,7 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="B7" s="452">
         <f>'Shares non-e FD subsectors'!E51</f>
@@ -27188,7 +27027,7 @@
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="B8" s="452">
         <f>'Shares non-e FD subsectors'!E52</f>
@@ -27197,7 +27036,7 @@
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="B9" s="452">
         <f>'Shares non-e FD subsectors'!E53</f>
@@ -27206,7 +27045,7 @@
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="B10" s="452">
         <f>'Shares non-e FD subsectors'!E54</f>
@@ -27215,7 +27054,7 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="B11" s="452">
         <f>'Shares non-e FD subsectors'!E55</f>
@@ -27224,7 +27063,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="B12" s="452">
         <f>'Shares non-e FD subsectors'!E56</f>
@@ -27680,10 +27519,10 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="2:4" ht="79" customHeight="1">
-      <c r="B5" s="560" t="s">
+      <c r="B5" s="564" t="s">
         <v>319</v>
       </c>
-      <c r="C5" s="561"/>
+      <c r="C5" s="565"/>
     </row>
     <row r="6" spans="2:4" ht="16" thickBot="1">
       <c r="B6" s="8"/>
@@ -28383,11 +28222,11 @@
       <c r="O4" s="8"/>
     </row>
     <row r="5" spans="2:16">
-      <c r="B5" s="562" t="s">
+      <c r="B5" s="566" t="s">
         <v>337</v>
       </c>
-      <c r="C5" s="563"/>
-      <c r="D5" s="564"/>
+      <c r="C5" s="567"/>
+      <c r="D5" s="568"/>
       <c r="G5" s="510"/>
       <c r="I5" s="16"/>
       <c r="J5" s="8"/>
@@ -28398,9 +28237,9 @@
       <c r="O5" s="8"/>
     </row>
     <row r="6" spans="2:16">
-      <c r="B6" s="562"/>
-      <c r="C6" s="563"/>
-      <c r="D6" s="564"/>
+      <c r="B6" s="566"/>
+      <c r="C6" s="567"/>
+      <c r="D6" s="568"/>
       <c r="G6" s="511"/>
       <c r="I6" s="16"/>
       <c r="J6" s="8"/>
@@ -28411,9 +28250,9 @@
       <c r="O6" s="8"/>
     </row>
     <row r="7" spans="2:16" ht="32" customHeight="1">
-      <c r="B7" s="560"/>
-      <c r="C7" s="565"/>
-      <c r="D7" s="561"/>
+      <c r="B7" s="564"/>
+      <c r="C7" s="569"/>
+      <c r="D7" s="565"/>
       <c r="I7" s="17"/>
       <c r="J7" s="10"/>
       <c r="K7" s="507"/>
@@ -29362,7 +29201,7 @@
         <v>242</v>
       </c>
       <c r="E47" s="339">
-        <f>'Non-energetic cons analysis'!D21</f>
+        <f>'Non-energetic cons analysis'!D19</f>
         <v>0</v>
       </c>
       <c r="F47" s="225"/>
@@ -29394,7 +29233,7 @@
         <v>242</v>
       </c>
       <c r="E48" s="339">
-        <f>'Non-energetic cons analysis'!G21</f>
+        <f>'Non-energetic cons analysis'!G19</f>
         <v>0</v>
       </c>
       <c r="F48" s="225"/>
@@ -29426,7 +29265,7 @@
         <v>242</v>
       </c>
       <c r="E49" s="339">
-        <f>'Non-energetic cons analysis'!H21</f>
+        <f>'Non-energetic cons analysis'!H19</f>
         <v>0</v>
       </c>
       <c r="F49" s="225"/>
@@ -29458,7 +29297,7 @@
         <v>242</v>
       </c>
       <c r="E50" s="339">
-        <f>'Non-energetic cons analysis'!I21</f>
+        <f>'Non-energetic cons analysis'!I19</f>
         <v>0</v>
       </c>
       <c r="F50" s="225"/>
@@ -29490,7 +29329,7 @@
         <v>242</v>
       </c>
       <c r="E51" s="339">
-        <f>'Non-energetic cons analysis'!J21</f>
+        <f>'Non-energetic cons analysis'!J19</f>
         <v>0</v>
       </c>
       <c r="F51" s="225"/>
@@ -29522,7 +29361,7 @@
         <v>242</v>
       </c>
       <c r="E52" s="339">
-        <f>'Non-energetic cons analysis'!K21</f>
+        <f>'Non-energetic cons analysis'!K19</f>
         <v>0</v>
       </c>
       <c r="F52" s="225"/>
@@ -29765,7 +29604,7 @@
         <v>242</v>
       </c>
       <c r="E64" s="523">
-        <f>'Non-energetic cons analysis'!L21</f>
+        <f>'Non-energetic cons analysis'!L19</f>
         <v>0</v>
       </c>
       <c r="F64" s="524"/>
@@ -29777,7 +29616,7 @@
         <v>506</v>
       </c>
       <c r="L64" s="520" t="e">
-        <f>'Non-energetic cons analysis'!L21/SUM('Non-energetic cons analysis'!D21:L21)</f>
+        <f>'Non-energetic cons analysis'!L19/SUM('Non-energetic cons analysis'!D19:L19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M64" s="214"/>
@@ -36920,13 +36759,13 @@
     </row>
     <row r="5" spans="1:17" ht="30" customHeight="1">
       <c r="A5" s="76"/>
-      <c r="B5" s="566" t="s">
+      <c r="B5" s="570" t="s">
         <v>474</v>
       </c>
-      <c r="C5" s="567"/>
-      <c r="D5" s="567"/>
-      <c r="E5" s="567"/>
-      <c r="F5" s="568"/>
+      <c r="C5" s="571"/>
+      <c r="D5" s="571"/>
+      <c r="E5" s="571"/>
+      <c r="F5" s="572"/>
       <c r="H5" s="76"/>
       <c r="I5" s="76"/>
       <c r="J5" s="76"/>

</xml_diff>

<commit_message>
Published state of ETDataset on February 20 2020
</commit_message>
<xml_diff>
--- a/analyses/5_industry_analysis.xlsx
+++ b/analyses/5_industry_analysis.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/roosdekok/Projects/etdataset/analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/etdataset/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3249BCA2-366B-994F-8482-F41D880A962C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A3BB46-85B7-2744-80D2-72C4DD3657C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="47280" windowHeight="25420" tabRatio="835" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28340" tabRatio="835" firstSheet="44" activeTab="54" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -64,10 +64,14 @@
     <sheet name="csv_industry_other_wood_non_e" sheetId="113" r:id="rId49"/>
     <sheet name="csv_industry_other_food_elec_ps" sheetId="115" r:id="rId50"/>
     <sheet name="csv_industry_other_paper_el_ps" sheetId="116" r:id="rId51"/>
+    <sheet name="csv_chemicals_other_residual_he" sheetId="117" r:id="rId52"/>
+    <sheet name="csv_refineries_residual_heat" sheetId="118" r:id="rId53"/>
+    <sheet name="csv_fertilizers_residual_heat" sheetId="119" r:id="rId54"/>
+    <sheet name="csv_ict_residual_heat" sheetId="121" r:id="rId55"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId52"/>
-    <externalReference r:id="rId53"/>
+    <externalReference r:id="rId56"/>
+    <externalReference r:id="rId57"/>
   </externalReferences>
   <definedNames>
     <definedName name="base_year" localSheetId="22">Dashboard!$E$14</definedName>
@@ -270,7 +274,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1287" uniqueCount="654">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1351" uniqueCount="687">
   <si>
     <t>Changelog</t>
   </si>
@@ -2310,7 +2314,106 @@
     <t>industry_electric_heater</t>
   </si>
   <si>
-    <t>Aggregated all industry other categories except for food and paper to non_specified. Caution to prevent confusion: the category non_specified was already used as one of the industry other subsectors. In this update, we merge all other categories (except food and paper, so: minerals, mining, etc.) into this non_specified category in the output csv tabs.</t>
+    <t>Residual heat</t>
+  </si>
+  <si>
+    <t>In the ETM residual heat is implemented as useful demand heat that is reused in heat networks. There are two types of residual heat distinguished: from flue gasses and processes. For each industrial sector the potential of these types can be chosen.</t>
+  </si>
+  <si>
+    <t>Residual heat from flue gasses</t>
+  </si>
+  <si>
+    <t>Residual heat from processes</t>
+  </si>
+  <si>
+    <t>Heat that cannot be recovered</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Residual heat potentials are added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residual heat from chemical sector [% of useful heat demand] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residual heat from fertilizer industry [% of useful heat demand] </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residual heat from refineries [% of useful heat demand] </t>
+  </si>
+  <si>
+    <t>residual_heat_processes_chemicals_other</t>
+  </si>
+  <si>
+    <t>residual_heat_flue_gasses_chemicals_other</t>
+  </si>
+  <si>
+    <t>residual_heat_flue_gasses_chemicals_refineries</t>
+  </si>
+  <si>
+    <t>residual_heat_processes_chemicals_refineries</t>
+  </si>
+  <si>
+    <t>residual_heat_flue_gasses_chemicals_fertilizers</t>
+  </si>
+  <si>
+    <t>residual_heat_processes_chemicals_fertilizers</t>
+  </si>
+  <si>
+    <t>industry_useful_demand_for_chemical_other_useable_heat_parent_share</t>
+  </si>
+  <si>
+    <t>industry_chemicals_other_flue_gasses_potential_residual_heat</t>
+  </si>
+  <si>
+    <t>industry_chemicals_other_processes_potential_residual_heat</t>
+  </si>
+  <si>
+    <t>industry_chemicals_other_used_heat</t>
+  </si>
+  <si>
+    <t>industry_useful_demand_for_chemical_refineries_useable_heat_parent_share</t>
+  </si>
+  <si>
+    <t>industry_chemicals_refineries_flue_gasses_potential_residual_heat</t>
+  </si>
+  <si>
+    <t>industry_chemicals_refineries_processes_potential_residual_heat</t>
+  </si>
+  <si>
+    <t>industry_chemicals_refineries_used_heat</t>
+  </si>
+  <si>
+    <t>industry_chemicals_fertilizers_flue_gasses_potential_residual_heat</t>
+  </si>
+  <si>
+    <t>industry_chemicals_fertilizers_processes_potential_residual_heat</t>
+  </si>
+  <si>
+    <t>industry_chemicals_fertilizers_used_heat</t>
+  </si>
+  <si>
+    <t>industry_useful_demand_for_other_ict_electricity_parent_share</t>
+  </si>
+  <si>
+    <t>industry_other_ict_potential_residual_heat_from_servers_electricity</t>
+  </si>
+  <si>
+    <t>industry_other_ict_other_systems_electricity</t>
+  </si>
+  <si>
+    <t>Residual heat from servers</t>
+  </si>
+  <si>
+    <t>residual_heat_ict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Residual heat from ICT [% of useful electricity demand] </t>
+  </si>
+  <si>
+    <t>industry_chemicals_fertilizers_haber_bosch_process_hydrogen_parent_share</t>
   </si>
 </sst>
 </file>
@@ -2652,7 +2755,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -3289,6 +3392,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1528">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -4820,7 +4936,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="610">
+  <cellXfs count="614">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -5974,6 +6090,11 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="54" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6046,7 +6167,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1528">
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
@@ -14277,7 +14397,7 @@
       </c>
       <c r="C8" s="71">
         <f>MAX(Changelog!B:B)</f>
-        <v>43864</v>
+        <v>43872</v>
       </c>
       <c r="D8" s="7"/>
     </row>
@@ -14562,13 +14682,13 @@
     </row>
     <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="76"/>
-      <c r="B5" s="591" t="s">
+      <c r="B5" s="596" t="s">
         <v>475</v>
       </c>
-      <c r="C5" s="592"/>
-      <c r="D5" s="592"/>
-      <c r="E5" s="592"/>
-      <c r="F5" s="593"/>
+      <c r="C5" s="597"/>
+      <c r="D5" s="597"/>
+      <c r="E5" s="597"/>
+      <c r="F5" s="598"/>
       <c r="H5" s="76"/>
       <c r="I5" s="76"/>
       <c r="J5" s="76"/>
@@ -15064,11 +15184,11 @@
       <c r="E4" s="84"/>
     </row>
     <row r="5" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="594" t="s">
+      <c r="B5" s="599" t="s">
         <v>479</v>
       </c>
-      <c r="C5" s="595"/>
-      <c r="D5" s="595"/>
+      <c r="C5" s="600"/>
+      <c r="D5" s="600"/>
       <c r="E5" s="84"/>
     </row>
     <row r="6" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -15247,12 +15367,12 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="596" t="s">
+      <c r="B5" s="601" t="s">
         <v>527</v>
       </c>
-      <c r="C5" s="597"/>
-      <c r="D5" s="597"/>
-      <c r="E5" s="598"/>
+      <c r="C5" s="602"/>
+      <c r="D5" s="602"/>
+      <c r="E5" s="603"/>
     </row>
     <row r="6" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
@@ -15719,12 +15839,12 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="2:5" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="596" t="s">
+      <c r="B5" s="601" t="s">
         <v>528</v>
       </c>
-      <c r="C5" s="597"/>
-      <c r="D5" s="597"/>
-      <c r="E5" s="598"/>
+      <c r="C5" s="602"/>
+      <c r="D5" s="602"/>
+      <c r="E5" s="603"/>
     </row>
     <row r="6" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
@@ -15986,14 +16106,14 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:12" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="594" t="s">
+      <c r="B5" s="599" t="s">
         <v>529</v>
       </c>
-      <c r="C5" s="595"/>
-      <c r="D5" s="595"/>
-      <c r="E5" s="595"/>
-      <c r="F5" s="595"/>
-      <c r="G5" s="599"/>
+      <c r="C5" s="600"/>
+      <c r="D5" s="600"/>
+      <c r="E5" s="600"/>
+      <c r="F5" s="600"/>
+      <c r="G5" s="604"/>
     </row>
     <row r="6" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -16717,14 +16837,14 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="2:12" ht="44" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="594" t="s">
+      <c r="B5" s="599" t="s">
         <v>622</v>
       </c>
-      <c r="C5" s="595"/>
-      <c r="D5" s="595"/>
-      <c r="E5" s="595"/>
-      <c r="F5" s="595"/>
-      <c r="G5" s="599"/>
+      <c r="C5" s="600"/>
+      <c r="D5" s="600"/>
+      <c r="E5" s="600"/>
+      <c r="F5" s="600"/>
+      <c r="G5" s="604"/>
     </row>
     <row r="6" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
@@ -17057,14 +17177,14 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="594" t="s">
+      <c r="B5" s="599" t="s">
         <v>530</v>
       </c>
-      <c r="C5" s="595"/>
-      <c r="D5" s="595"/>
-      <c r="E5" s="595"/>
-      <c r="F5" s="595"/>
-      <c r="G5" s="599"/>
+      <c r="C5" s="600"/>
+      <c r="D5" s="600"/>
+      <c r="E5" s="600"/>
+      <c r="F5" s="600"/>
+      <c r="G5" s="604"/>
     </row>
     <row r="6" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
@@ -17592,7 +17712,7 @@
   <dimension ref="B2:L22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17635,14 +17755,14 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="594" t="s">
+      <c r="B5" s="599" t="s">
         <v>531</v>
       </c>
-      <c r="C5" s="595"/>
-      <c r="D5" s="595"/>
-      <c r="E5" s="595"/>
-      <c r="F5" s="595"/>
-      <c r="G5" s="599"/>
+      <c r="C5" s="600"/>
+      <c r="D5" s="600"/>
+      <c r="E5" s="600"/>
+      <c r="F5" s="600"/>
+      <c r="G5" s="604"/>
     </row>
     <row r="6" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
@@ -18087,7 +18207,7 @@
   <dimension ref="A2:L28"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18129,14 +18249,14 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="2:12" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="594" t="s">
+      <c r="B5" s="599" t="s">
         <v>532</v>
       </c>
-      <c r="C5" s="595"/>
-      <c r="D5" s="595"/>
-      <c r="E5" s="595"/>
-      <c r="F5" s="595"/>
-      <c r="G5" s="599"/>
+      <c r="C5" s="600"/>
+      <c r="D5" s="600"/>
+      <c r="E5" s="600"/>
+      <c r="F5" s="600"/>
+      <c r="G5" s="604"/>
     </row>
     <row r="6" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
@@ -18769,7 +18889,7 @@
   </sheetPr>
   <dimension ref="A2:L20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -18813,14 +18933,14 @@
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="594" t="s">
+      <c r="B5" s="599" t="s">
         <v>533</v>
       </c>
-      <c r="C5" s="595"/>
-      <c r="D5" s="595"/>
-      <c r="E5" s="595"/>
-      <c r="F5" s="595"/>
-      <c r="G5" s="599"/>
+      <c r="C5" s="600"/>
+      <c r="D5" s="600"/>
+      <c r="E5" s="600"/>
+      <c r="F5" s="600"/>
+      <c r="G5" s="604"/>
     </row>
     <row r="6" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:12" x14ac:dyDescent="0.2">
@@ -19144,10 +19264,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="2"/>
   </sheetPr>
-  <dimension ref="B2:D62"/>
+  <dimension ref="B2:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D70" sqref="D70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19785,21 +19905,31 @@
         <v>1.52</v>
       </c>
     </row>
-    <row r="61" spans="2:4" ht="119" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" s="156">
-        <v>43864</v>
-      </c>
-      <c r="C61" s="158" t="s">
-        <v>653</v>
+        <v>43872</v>
+      </c>
+      <c r="C61" s="157" t="s">
+        <v>659</v>
       </c>
       <c r="D61" s="159">
         <v>1.53</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B62" s="609"/>
-      <c r="C62" s="10"/>
-      <c r="D62" s="254"/>
+      <c r="B62" s="156"/>
+      <c r="C62" s="157"/>
+      <c r="D62" s="159"/>
+    </row>
+    <row r="63" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B63" s="156"/>
+      <c r="C63" s="157"/>
+      <c r="D63" s="159"/>
+    </row>
+    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B64" s="17"/>
+      <c r="C64" s="10"/>
+      <c r="D64" s="254"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -19862,11 +19992,11 @@
       <c r="E4" s="8"/>
     </row>
     <row r="5" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="600" t="s">
+      <c r="B5" s="605" t="s">
         <v>363</v>
       </c>
-      <c r="C5" s="601"/>
-      <c r="D5" s="602"/>
+      <c r="C5" s="606"/>
+      <c r="D5" s="607"/>
       <c r="E5" s="167"/>
     </row>
     <row r="6" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -20093,15 +20223,15 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="2:13" ht="90" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="603" t="s">
+      <c r="B5" s="608" t="s">
         <v>513</v>
       </c>
-      <c r="C5" s="604"/>
-      <c r="D5" s="604"/>
-      <c r="E5" s="604"/>
-      <c r="F5" s="604"/>
-      <c r="G5" s="604"/>
-      <c r="H5" s="605"/>
+      <c r="C5" s="609"/>
+      <c r="D5" s="609"/>
+      <c r="E5" s="609"/>
+      <c r="F5" s="609"/>
+      <c r="G5" s="609"/>
+      <c r="H5" s="610"/>
     </row>
     <row r="6" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
@@ -20693,7 +20823,7 @@
   <dimension ref="B2:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -20739,15 +20869,15 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="2:13" ht="55" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="606" t="s">
+      <c r="B5" s="611" t="s">
         <v>618</v>
       </c>
-      <c r="C5" s="607"/>
-      <c r="D5" s="607"/>
-      <c r="E5" s="607"/>
-      <c r="F5" s="607"/>
-      <c r="G5" s="607"/>
-      <c r="H5" s="608"/>
+      <c r="C5" s="612"/>
+      <c r="D5" s="612"/>
+      <c r="E5" s="612"/>
+      <c r="F5" s="612"/>
+      <c r="G5" s="612"/>
+      <c r="H5" s="613"/>
     </row>
     <row r="6" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
@@ -21504,7 +21634,7 @@
   <dimension ref="A2:M27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -21551,15 +21681,15 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:13" ht="60" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="606" t="s">
+      <c r="B5" s="611" t="s">
         <v>620</v>
       </c>
-      <c r="C5" s="607"/>
-      <c r="D5" s="607"/>
-      <c r="E5" s="607"/>
-      <c r="F5" s="607"/>
-      <c r="G5" s="607"/>
-      <c r="H5" s="608"/>
+      <c r="C5" s="612"/>
+      <c r="D5" s="612"/>
+      <c r="E5" s="612"/>
+      <c r="F5" s="612"/>
+      <c r="G5" s="612"/>
+      <c r="H5" s="613"/>
     </row>
     <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -22304,7 +22434,7 @@
   <dimension ref="A2:M29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22351,15 +22481,15 @@
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:13" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="594" t="s">
+      <c r="B5" s="599" t="s">
         <v>619</v>
       </c>
-      <c r="C5" s="595"/>
-      <c r="D5" s="595"/>
-      <c r="E5" s="595"/>
-      <c r="F5" s="595"/>
-      <c r="G5" s="595"/>
-      <c r="H5" s="599"/>
+      <c r="C5" s="600"/>
+      <c r="D5" s="600"/>
+      <c r="E5" s="600"/>
+      <c r="F5" s="600"/>
+      <c r="G5" s="600"/>
+      <c r="H5" s="604"/>
     </row>
     <row r="6" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
@@ -23018,8 +23148,8 @@
   </sheetPr>
   <dimension ref="B2:G93"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H28" sqref="H28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D78" sqref="D78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23046,12 +23176,12 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="596" t="s">
+      <c r="B5" s="601" t="s">
         <v>484</v>
       </c>
-      <c r="C5" s="597"/>
-      <c r="D5" s="597"/>
-      <c r="E5" s="598"/>
+      <c r="C5" s="602"/>
+      <c r="D5" s="602"/>
+      <c r="E5" s="603"/>
     </row>
     <row r="6" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
@@ -24284,12 +24414,12 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B5" s="596" t="s">
+      <c r="B5" s="601" t="s">
         <v>484</v>
       </c>
-      <c r="C5" s="597"/>
-      <c r="D5" s="597"/>
-      <c r="E5" s="598"/>
+      <c r="C5" s="602"/>
+      <c r="D5" s="602"/>
+      <c r="E5" s="603"/>
     </row>
     <row r="6" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
@@ -25522,12 +25652,12 @@
       <c r="E4" s="5"/>
     </row>
     <row r="5" spans="2:7" ht="31" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="596" t="s">
+      <c r="B5" s="601" t="s">
         <v>638</v>
       </c>
-      <c r="C5" s="597"/>
-      <c r="D5" s="597"/>
-      <c r="E5" s="598"/>
+      <c r="C5" s="602"/>
+      <c r="D5" s="602"/>
+      <c r="E5" s="603"/>
     </row>
     <row r="6" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="7" spans="2:7" x14ac:dyDescent="0.2">
@@ -25833,7 +25963,7 @@
   </sheetPr>
   <dimension ref="B2:C59"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -26830,9 +26960,7 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -27066,7 +27194,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -27133,12 +27261,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -27200,12 +27328,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="I71" sqref="I71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -27267,12 +27395,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="64.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -27334,12 +27462,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -27401,12 +27529,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="65.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="66.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -27468,12 +27596,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="73.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="60.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -27535,12 +27663,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="70" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="46.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -27602,12 +27730,12 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="73.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -27670,7 +27798,7 @@
   <dimension ref="B2:CZ29"/>
   <sheetViews>
     <sheetView topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="BE52" sqref="BE52"/>
+      <selection activeCell="CO17" sqref="CO17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -28148,13 +28276,10 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="55.5" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -28230,12 +28355,12 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="AB60" sqref="AB60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="56.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -28301,6 +28426,239 @@
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B71940-1AD1-E440-9192-65CCF3B5FCDE}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>670</v>
+      </c>
+      <c r="B3" s="452">
+        <f>Dashboard!E85</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>671</v>
+      </c>
+      <c r="B4" s="452">
+        <f>Dashboard!E86</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>672</v>
+      </c>
+      <c r="B5" s="452">
+        <f>Dashboard!E87</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C6FF57E-AC00-A144-98DC-C9E113E51D8D}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>674</v>
+      </c>
+      <c r="B3" s="452">
+        <f>Dashboard!E90</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>675</v>
+      </c>
+      <c r="B4" s="452">
+        <f>Dashboard!E91</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>676</v>
+      </c>
+      <c r="B5" s="452">
+        <f>Dashboard!E92</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0859CC87-3D21-F24F-9F38-432043B5D750}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>677</v>
+      </c>
+      <c r="B3" s="452">
+        <f>Dashboard!E95</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>678</v>
+      </c>
+      <c r="B4" s="452">
+        <f>Dashboard!E96</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>679</v>
+      </c>
+      <c r="B5" s="452">
+        <f>Dashboard!E97</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A8EDABB-E71D-8A48-AE17-655974A88DE1}">
+  <sheetPr>
+    <tabColor theme="7" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="45.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>681</v>
+      </c>
+      <c r="B3" s="452">
+        <f>Dashboard!E100</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>682</v>
+      </c>
+      <c r="B4" s="452">
+        <f>Dashboard!E101</f>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -28335,10 +28693,10 @@
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="2:4" ht="79" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="585" t="s">
+      <c r="B5" s="590" t="s">
         <v>319</v>
       </c>
-      <c r="C5" s="586"/>
+      <c r="C5" s="591"/>
     </row>
     <row r="6" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
@@ -28968,10 +29326,10 @@
   <sheetPr codeName="Sheet7">
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
-  <dimension ref="B2:P77"/>
+  <dimension ref="B2:P102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="K98" sqref="K98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -29040,11 +29398,11 @@
       <c r="O4" s="8"/>
     </row>
     <row r="5" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B5" s="587" t="s">
+      <c r="B5" s="592" t="s">
         <v>337</v>
       </c>
-      <c r="C5" s="588"/>
-      <c r="D5" s="589"/>
+      <c r="C5" s="593"/>
+      <c r="D5" s="594"/>
       <c r="G5" s="510"/>
       <c r="I5" s="16"/>
       <c r="J5" s="8"/>
@@ -29055,9 +29413,9 @@
       <c r="O5" s="8"/>
     </row>
     <row r="6" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="B6" s="587"/>
-      <c r="C6" s="588"/>
-      <c r="D6" s="589"/>
+      <c r="B6" s="592"/>
+      <c r="C6" s="593"/>
+      <c r="D6" s="594"/>
       <c r="G6" s="511"/>
       <c r="I6" s="16"/>
       <c r="J6" s="8"/>
@@ -29068,9 +29426,9 @@
       <c r="O6" s="8"/>
     </row>
     <row r="7" spans="2:16" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="585"/>
-      <c r="C7" s="590"/>
-      <c r="D7" s="586"/>
+      <c r="B7" s="590"/>
+      <c r="C7" s="595"/>
+      <c r="D7" s="591"/>
       <c r="I7" s="17"/>
       <c r="J7" s="10"/>
       <c r="K7" s="507"/>
@@ -30724,6 +31082,469 @@
       <c r="M77" s="218"/>
       <c r="O77" s="322"/>
       <c r="P77" s="325"/>
+    </row>
+    <row r="79" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="250" t="s">
+        <v>653</v>
+      </c>
+      <c r="C80" s="246"/>
+      <c r="D80" s="248"/>
+      <c r="E80" s="246"/>
+      <c r="F80" s="246"/>
+      <c r="G80" s="246"/>
+      <c r="H80" s="246"/>
+      <c r="I80" s="246"/>
+      <c r="J80" s="246"/>
+      <c r="K80" s="246"/>
+      <c r="L80" s="246"/>
+      <c r="M80" s="249"/>
+      <c r="O80" s="586"/>
+      <c r="P80" s="5"/>
+    </row>
+    <row r="81" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B81" s="585"/>
+      <c r="C81" s="43"/>
+      <c r="D81" s="92"/>
+      <c r="E81" s="43"/>
+      <c r="F81" s="43"/>
+      <c r="G81" s="43"/>
+      <c r="H81" s="43"/>
+      <c r="I81" s="43"/>
+      <c r="J81" s="43"/>
+      <c r="K81" s="43"/>
+      <c r="L81" s="43"/>
+      <c r="M81" s="26"/>
+      <c r="O81" s="16"/>
+      <c r="P81" s="7"/>
+    </row>
+    <row r="82" spans="2:16" ht="85" x14ac:dyDescent="0.2">
+      <c r="B82" s="27"/>
+      <c r="C82" s="240" t="s">
+        <v>654</v>
+      </c>
+      <c r="D82" s="94"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="8"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="8"/>
+      <c r="I82" s="8"/>
+      <c r="J82" s="8"/>
+      <c r="K82" s="8"/>
+      <c r="L82" s="8"/>
+      <c r="M82" s="28"/>
+      <c r="O82" s="16"/>
+      <c r="P82" s="7"/>
+    </row>
+    <row r="83" spans="2:16" s="49" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B83" s="284" t="s">
+        <v>375</v>
+      </c>
+      <c r="C83" s="285"/>
+      <c r="D83" s="286" t="s">
+        <v>86</v>
+      </c>
+      <c r="E83" s="346" t="s">
+        <v>85</v>
+      </c>
+      <c r="F83" s="287"/>
+      <c r="G83" s="287"/>
+      <c r="H83" s="287"/>
+      <c r="I83" s="277"/>
+      <c r="J83" s="277"/>
+      <c r="K83" s="281" t="s">
+        <v>87</v>
+      </c>
+      <c r="L83" s="277" t="s">
+        <v>88</v>
+      </c>
+      <c r="M83" s="288" t="s">
+        <v>83</v>
+      </c>
+      <c r="O83" s="323"/>
+      <c r="P83" s="324"/>
+    </row>
+    <row r="84" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="33" t="s">
+        <v>660</v>
+      </c>
+      <c r="C84" s="8"/>
+      <c r="D84" s="94"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="8"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="8"/>
+      <c r="I84" s="8"/>
+      <c r="J84" s="8"/>
+      <c r="K84" s="8"/>
+      <c r="L84" s="8"/>
+      <c r="M84" s="28"/>
+      <c r="O84" s="16"/>
+      <c r="P84" s="7"/>
+    </row>
+    <row r="85" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="27"/>
+      <c r="C85" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="D85" s="94" t="s">
+        <v>658</v>
+      </c>
+      <c r="E85" s="587"/>
+      <c r="F85" s="8"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="20"/>
+      <c r="J85" s="8"/>
+      <c r="K85" s="8"/>
+      <c r="L85" s="8"/>
+      <c r="M85" s="28"/>
+      <c r="O85" s="317" t="s">
+        <v>664</v>
+      </c>
+      <c r="P85" s="7"/>
+    </row>
+    <row r="86" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B86" s="27"/>
+      <c r="C86" s="8" t="s">
+        <v>656</v>
+      </c>
+      <c r="D86" s="94" t="s">
+        <v>658</v>
+      </c>
+      <c r="E86" s="588"/>
+      <c r="F86" s="8"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="8"/>
+      <c r="I86" s="20"/>
+      <c r="J86" s="8"/>
+      <c r="K86" s="8"/>
+      <c r="L86" s="8"/>
+      <c r="M86" s="28"/>
+      <c r="O86" s="317" t="s">
+        <v>663</v>
+      </c>
+      <c r="P86" s="7"/>
+    </row>
+    <row r="87" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B87" s="27"/>
+      <c r="C87" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="D87" s="94" t="s">
+        <v>658</v>
+      </c>
+      <c r="E87" s="589">
+        <f>1-E85-E86</f>
+        <v>1</v>
+      </c>
+      <c r="F87" s="8"/>
+      <c r="G87" s="8"/>
+      <c r="H87" s="8"/>
+      <c r="I87" s="8"/>
+      <c r="J87" s="8"/>
+      <c r="K87" s="8"/>
+      <c r="L87" s="8"/>
+      <c r="M87" s="28"/>
+      <c r="O87" s="16"/>
+      <c r="P87" s="7"/>
+    </row>
+    <row r="88" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B88" s="27"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="94"/>
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
+      <c r="G88" s="8"/>
+      <c r="H88" s="8"/>
+      <c r="I88" s="8"/>
+      <c r="J88" s="8"/>
+      <c r="K88" s="8"/>
+      <c r="L88" s="8"/>
+      <c r="M88" s="28"/>
+      <c r="O88" s="16"/>
+      <c r="P88" s="7"/>
+    </row>
+    <row r="89" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B89" s="33" t="s">
+        <v>662</v>
+      </c>
+      <c r="C89" s="8"/>
+      <c r="D89" s="94"/>
+      <c r="E89" s="8"/>
+      <c r="F89" s="8"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="8"/>
+      <c r="I89" s="8"/>
+      <c r="J89" s="8"/>
+      <c r="K89" s="8"/>
+      <c r="L89" s="8"/>
+      <c r="M89" s="28"/>
+      <c r="O89" s="16"/>
+      <c r="P89" s="7"/>
+    </row>
+    <row r="90" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B90" s="27"/>
+      <c r="C90" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="D90" s="94" t="s">
+        <v>658</v>
+      </c>
+      <c r="E90" s="587"/>
+      <c r="F90" s="8"/>
+      <c r="G90" s="8"/>
+      <c r="H90" s="8"/>
+      <c r="I90" s="20"/>
+      <c r="J90" s="8"/>
+      <c r="K90" s="8"/>
+      <c r="L90" s="8"/>
+      <c r="M90" s="28"/>
+      <c r="O90" s="317" t="s">
+        <v>665</v>
+      </c>
+      <c r="P90" s="7"/>
+    </row>
+    <row r="91" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B91" s="27"/>
+      <c r="C91" s="8" t="s">
+        <v>656</v>
+      </c>
+      <c r="D91" s="94" t="s">
+        <v>658</v>
+      </c>
+      <c r="E91" s="588"/>
+      <c r="F91" s="8"/>
+      <c r="G91" s="8"/>
+      <c r="H91" s="8"/>
+      <c r="I91" s="20"/>
+      <c r="J91" s="8"/>
+      <c r="K91" s="8"/>
+      <c r="L91" s="8"/>
+      <c r="M91" s="28"/>
+      <c r="O91" s="317" t="s">
+        <v>666</v>
+      </c>
+      <c r="P91" s="7"/>
+    </row>
+    <row r="92" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B92" s="27"/>
+      <c r="C92" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="D92" s="94" t="s">
+        <v>658</v>
+      </c>
+      <c r="E92" s="589">
+        <f>1-E90-E91</f>
+        <v>1</v>
+      </c>
+      <c r="F92" s="8"/>
+      <c r="G92" s="8"/>
+      <c r="H92" s="8"/>
+      <c r="I92" s="8"/>
+      <c r="J92" s="8"/>
+      <c r="K92" s="8"/>
+      <c r="L92" s="8"/>
+      <c r="M92" s="28"/>
+      <c r="O92" s="16"/>
+      <c r="P92" s="7"/>
+    </row>
+    <row r="93" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B93" s="27"/>
+      <c r="C93" s="8"/>
+      <c r="D93" s="94"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="8"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="8"/>
+      <c r="I93" s="8"/>
+      <c r="J93" s="8"/>
+      <c r="K93" s="8"/>
+      <c r="L93" s="8"/>
+      <c r="M93" s="28"/>
+      <c r="O93" s="16"/>
+      <c r="P93" s="7"/>
+    </row>
+    <row r="94" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B94" s="33" t="s">
+        <v>661</v>
+      </c>
+      <c r="C94" s="8"/>
+      <c r="D94" s="94"/>
+      <c r="E94" s="8"/>
+      <c r="F94" s="8"/>
+      <c r="G94" s="8"/>
+      <c r="H94" s="8"/>
+      <c r="I94" s="8"/>
+      <c r="J94" s="8"/>
+      <c r="K94" s="8"/>
+      <c r="L94" s="8"/>
+      <c r="M94" s="28"/>
+      <c r="O94" s="16"/>
+      <c r="P94" s="7"/>
+    </row>
+    <row r="95" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B95" s="27"/>
+      <c r="C95" s="8" t="s">
+        <v>655</v>
+      </c>
+      <c r="D95" s="94" t="s">
+        <v>658</v>
+      </c>
+      <c r="E95" s="587"/>
+      <c r="F95" s="8"/>
+      <c r="G95" s="8"/>
+      <c r="H95" s="8"/>
+      <c r="I95" s="20"/>
+      <c r="J95" s="8"/>
+      <c r="K95" s="8"/>
+      <c r="L95" s="8"/>
+      <c r="M95" s="28"/>
+      <c r="O95" s="317" t="s">
+        <v>667</v>
+      </c>
+      <c r="P95" s="7"/>
+    </row>
+    <row r="96" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B96" s="27"/>
+      <c r="C96" s="8" t="s">
+        <v>656</v>
+      </c>
+      <c r="D96" s="94" t="s">
+        <v>658</v>
+      </c>
+      <c r="E96" s="588"/>
+      <c r="F96" s="8"/>
+      <c r="G96" s="8"/>
+      <c r="H96" s="8"/>
+      <c r="I96" s="20"/>
+      <c r="J96" s="8"/>
+      <c r="K96" s="8"/>
+      <c r="L96" s="8"/>
+      <c r="M96" s="28"/>
+      <c r="O96" s="317" t="s">
+        <v>668</v>
+      </c>
+      <c r="P96" s="7"/>
+    </row>
+    <row r="97" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B97" s="27"/>
+      <c r="C97" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="D97" s="94" t="s">
+        <v>658</v>
+      </c>
+      <c r="E97" s="589">
+        <f>1-E95-E96</f>
+        <v>1</v>
+      </c>
+      <c r="F97" s="8"/>
+      <c r="G97" s="8"/>
+      <c r="H97" s="8"/>
+      <c r="I97" s="8"/>
+      <c r="J97" s="8"/>
+      <c r="K97" s="8"/>
+      <c r="L97" s="8"/>
+      <c r="M97" s="28"/>
+      <c r="O97" s="16"/>
+      <c r="P97" s="7"/>
+    </row>
+    <row r="98" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B98" s="27"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="94"/>
+      <c r="E98" s="8"/>
+      <c r="F98" s="8"/>
+      <c r="G98" s="8"/>
+      <c r="H98" s="8"/>
+      <c r="I98" s="8"/>
+      <c r="J98" s="8"/>
+      <c r="K98" s="8"/>
+      <c r="L98" s="8"/>
+      <c r="M98" s="28"/>
+      <c r="O98" s="16"/>
+      <c r="P98" s="7"/>
+    </row>
+    <row r="99" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B99" s="33" t="s">
+        <v>685</v>
+      </c>
+      <c r="C99" s="8"/>
+      <c r="D99" s="94"/>
+      <c r="E99" s="8"/>
+      <c r="F99" s="8"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="8"/>
+      <c r="I99" s="8"/>
+      <c r="J99" s="8"/>
+      <c r="K99" s="8"/>
+      <c r="L99" s="8"/>
+      <c r="M99" s="28"/>
+      <c r="O99" s="16"/>
+      <c r="P99" s="7"/>
+    </row>
+    <row r="100" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B100" s="27"/>
+      <c r="C100" s="8" t="s">
+        <v>683</v>
+      </c>
+      <c r="D100" s="94" t="s">
+        <v>658</v>
+      </c>
+      <c r="E100" s="588"/>
+      <c r="F100" s="8"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="8"/>
+      <c r="I100" s="20"/>
+      <c r="J100" s="8"/>
+      <c r="K100" s="8"/>
+      <c r="L100" s="8"/>
+      <c r="M100" s="28"/>
+      <c r="O100" s="317" t="s">
+        <v>684</v>
+      </c>
+      <c r="P100" s="7"/>
+    </row>
+    <row r="101" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B101" s="27"/>
+      <c r="C101" s="8" t="s">
+        <v>657</v>
+      </c>
+      <c r="D101" s="94" t="s">
+        <v>658</v>
+      </c>
+      <c r="E101" s="589">
+        <f>1-E100</f>
+        <v>1</v>
+      </c>
+      <c r="F101" s="8"/>
+      <c r="G101" s="8"/>
+      <c r="H101" s="8"/>
+      <c r="I101" s="8"/>
+      <c r="J101" s="8"/>
+      <c r="K101" s="8"/>
+      <c r="L101" s="8"/>
+      <c r="M101" s="28"/>
+      <c r="O101" s="16"/>
+      <c r="P101" s="7"/>
+    </row>
+    <row r="102" spans="2:16" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B102" s="38"/>
+      <c r="C102" s="47"/>
+      <c r="D102" s="47"/>
+      <c r="E102" s="47"/>
+      <c r="F102" s="47"/>
+      <c r="G102" s="47"/>
+      <c r="H102" s="47"/>
+      <c r="I102" s="47"/>
+      <c r="J102" s="47"/>
+      <c r="K102" s="47"/>
+      <c r="L102" s="47"/>
+      <c r="M102" s="48"/>
+      <c r="O102" s="17"/>
+      <c r="P102" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -37854,13 +38675,13 @@
     </row>
     <row r="5" spans="1:17" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="76"/>
-      <c r="B5" s="591" t="s">
+      <c r="B5" s="596" t="s">
         <v>474</v>
       </c>
-      <c r="C5" s="592"/>
-      <c r="D5" s="592"/>
-      <c r="E5" s="592"/>
-      <c r="F5" s="593"/>
+      <c r="C5" s="597"/>
+      <c r="D5" s="597"/>
+      <c r="E5" s="597"/>
+      <c r="F5" s="598"/>
       <c r="H5" s="76"/>
       <c r="I5" s="76"/>
       <c r="J5" s="76"/>

</xml_diff>

<commit_message>
Published state of ETDataset for deploy August 2025
</commit_message>
<xml_diff>
--- a/analyses/5_industry_analysis.xlsx
+++ b/analyses/5_industry_analysis.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10608"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathijsbijkerk/Projects/etdataset/analyses/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mathijsbijkerk/Github/etdataset/analyses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC36558E-8886-F944-BF06-9E6562DB021F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56CDC1EC-F7CF-D944-851E-997FFF2A1A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12580" yWindow="-28300" windowWidth="51200" windowHeight="27160" tabRatio="835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7380" yWindow="-33340" windowWidth="30080" windowHeight="32380" tabRatio="835" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="34" r:id="rId1"/>
@@ -270,7 +270,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="656">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1272" uniqueCount="660">
   <si>
     <t>Changelog</t>
   </si>
@@ -2317,6 +2317,18 @@
   </si>
   <si>
     <t>nl</t>
+  </si>
+  <si>
+    <t>Naphtha (TJ)</t>
+  </si>
+  <si>
+    <t>Naptha (TJ)</t>
+  </si>
+  <si>
+    <t>July 1, 2025</t>
+  </si>
+  <si>
+    <t>Minor changes to allow naphtha split from crude oil in the industry sector. Only minimal changes are made to the analyses, so documentation is limited.</t>
   </si>
 </sst>
 </file>
@@ -14051,8 +14063,8 @@
   </sheetPr>
   <dimension ref="B2:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14084,7 +14096,7 @@
       </c>
       <c r="C5" s="22">
         <f>MAX(Changelog!D:D)</f>
-        <v>1.55</v>
+        <v>1.56</v>
       </c>
       <c r="D5" s="7"/>
     </row>
@@ -14111,7 +14123,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="68" t="s">
-        <v>652</v>
+        <v>658</v>
       </c>
       <c r="D8" s="7"/>
     </row>
@@ -15803,7 +15815,7 @@
   <dimension ref="A2:L29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16078,7 +16090,7 @@
         <v>0</v>
       </c>
       <c r="H14" s="406">
-        <f>-(SUM('Corrected energy balance step 2'!U49:AQ49)+SUM('Corrected energy balance step 2'!AW49:AZ49))</f>
+        <f>-(SUM('Corrected energy balance step 2'!U49:AQ49)+SUM('Corrected energy balance step 2'!AW49:AZ49))+'Corrected energy balance step 2'!AK49</f>
         <v>0</v>
       </c>
       <c r="I14" s="406">
@@ -16772,19 +16784,19 @@
         <v>0</v>
       </c>
       <c r="I11" s="406">
-        <f>'Non-energetic cons analysis'!I11</f>
+        <f>'Non-energetic cons analysis'!J11</f>
         <v>0</v>
       </c>
       <c r="J11" s="406">
-        <f>'Non-energetic cons analysis'!J11</f>
+        <f>'Non-energetic cons analysis'!K11</f>
         <v>0</v>
       </c>
       <c r="K11" s="406">
-        <f>'Non-energetic cons analysis'!K11</f>
+        <f>'Non-energetic cons analysis'!L11</f>
         <v>0</v>
       </c>
       <c r="L11" s="382">
-        <f>'Non-energetic cons analysis'!L11</f>
+        <f>'Non-energetic cons analysis'!M11</f>
         <v>0</v>
       </c>
     </row>
@@ -16814,19 +16826,19 @@
         <v>0</v>
       </c>
       <c r="I12" s="406">
-        <f>'Non-energetic cons analysis'!I14</f>
+        <f>'Non-energetic cons analysis'!J14</f>
         <v>0</v>
       </c>
       <c r="J12" s="406">
-        <f>'Non-energetic cons analysis'!J14</f>
+        <f>'Non-energetic cons analysis'!K14</f>
         <v>0</v>
       </c>
       <c r="K12" s="406">
-        <f>'Non-energetic cons analysis'!K14</f>
+        <f>'Non-energetic cons analysis'!L14</f>
         <v>0</v>
       </c>
       <c r="L12" s="382">
-        <f>'Non-energetic cons analysis'!L14</f>
+        <f>'Non-energetic cons analysis'!M14</f>
         <v>0</v>
       </c>
     </row>
@@ -16858,19 +16870,19 @@
         <v>0</v>
       </c>
       <c r="I13" s="387">
-        <f>'Non-energetic cons analysis'!I16</f>
+        <f>'Non-energetic cons analysis'!J16</f>
         <v>0</v>
       </c>
       <c r="J13" s="387">
-        <f>'Non-energetic cons analysis'!J16</f>
+        <f>'Non-energetic cons analysis'!K16</f>
         <v>0</v>
       </c>
       <c r="K13" s="387">
-        <f>'Non-energetic cons analysis'!K16</f>
+        <f>'Non-energetic cons analysis'!L16</f>
         <v>0</v>
       </c>
       <c r="L13" s="382">
-        <f>'Non-energetic cons analysis'!L16</f>
+        <f>'Non-energetic cons analysis'!M16</f>
         <v>0</v>
       </c>
     </row>
@@ -17678,19 +17690,19 @@
         <v>0</v>
       </c>
       <c r="I11" s="414">
-        <f>-'Fuel aggregation'!J15</f>
+        <f>-'Fuel aggregation'!K15</f>
         <v>0</v>
       </c>
       <c r="J11" s="414">
-        <f>-'Fuel aggregation'!K15</f>
+        <f>-'Fuel aggregation'!L15</f>
         <v>0</v>
       </c>
       <c r="K11" s="414">
-        <f>-'Fuel aggregation'!L15</f>
+        <f>-'Fuel aggregation'!M15</f>
         <v>0</v>
       </c>
       <c r="L11" s="416">
-        <f>-'Fuel aggregation'!M15</f>
+        <f>-'Fuel aggregation'!N15</f>
         <v>0</v>
       </c>
     </row>
@@ -17720,19 +17732,19 @@
         <v>0</v>
       </c>
       <c r="I12" s="414">
-        <f>-'Fuel aggregation'!J17</f>
+        <f>-'Fuel aggregation'!K17</f>
         <v>0</v>
       </c>
       <c r="J12" s="414">
-        <f>-'Fuel aggregation'!K17</f>
+        <f>-'Fuel aggregation'!L17</f>
         <v>0</v>
       </c>
       <c r="K12" s="414">
-        <f>-'Fuel aggregation'!L17</f>
+        <f>-'Fuel aggregation'!M17</f>
         <v>0</v>
       </c>
       <c r="L12" s="416">
-        <f>-'Fuel aggregation'!M17</f>
+        <f>-'Fuel aggregation'!N17</f>
         <v>0</v>
       </c>
     </row>
@@ -17764,19 +17776,19 @@
         <v>0</v>
       </c>
       <c r="I13" s="466">
-        <f>-'Fuel aggregation'!J16</f>
+        <f>-'Fuel aggregation'!K16</f>
         <v>0</v>
       </c>
       <c r="J13" s="466">
-        <f>-'Fuel aggregation'!K16</f>
+        <f>-'Fuel aggregation'!L16</f>
         <v>0</v>
       </c>
       <c r="K13" s="466">
-        <f>-'Fuel aggregation'!L16</f>
+        <f>-'Fuel aggregation'!M16</f>
         <v>0</v>
       </c>
       <c r="L13" s="467">
-        <f>-'Fuel aggregation'!M16</f>
+        <f>-'Fuel aggregation'!N16</f>
         <v>0</v>
       </c>
     </row>
@@ -18023,7 +18035,7 @@
   <dimension ref="A2:L28"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18173,19 +18185,19 @@
         <v>0</v>
       </c>
       <c r="I11" s="408">
-        <f>'Fuel aggregation'!J20</f>
+        <f>'Fuel aggregation'!K20</f>
         <v>0</v>
       </c>
       <c r="J11" s="408">
-        <f>'Fuel aggregation'!K20</f>
+        <f>'Fuel aggregation'!L20</f>
         <v>0</v>
       </c>
       <c r="K11" s="408">
-        <f>'Fuel aggregation'!L20</f>
+        <f>'Fuel aggregation'!M20</f>
         <v>0</v>
       </c>
       <c r="L11" s="421">
-        <f>'Fuel aggregation'!M20</f>
+        <f>'Fuel aggregation'!N20</f>
         <v>0</v>
       </c>
     </row>
@@ -18210,7 +18222,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="408">
-        <f>-SUM('Corrected energy balance step 2'!U49:AQ49)-SUM('Corrected energy balance step 2'!AW49:AZ49)</f>
+        <f>-SUM('Corrected energy balance step 2'!U49:AQ49)-SUM('Corrected energy balance step 2'!AW49:AZ49)+'Corrected energy balance step 2'!AK49</f>
         <v>0</v>
       </c>
       <c r="I12" s="408">
@@ -18707,10 +18719,10 @@
   <sheetPr codeName="Sheet19">
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="A2:L20"/>
+  <dimension ref="A2:M20"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18718,11 +18730,11 @@
     <col min="1" max="1" width="10.83203125" style="72"/>
     <col min="2" max="2" width="56.6640625" style="72" customWidth="1"/>
     <col min="3" max="3" width="2.83203125" style="193" customWidth="1"/>
-    <col min="4" max="12" width="15.83203125" style="72" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="72"/>
+    <col min="4" max="13" width="15.83203125" style="72" customWidth="1"/>
+    <col min="14" max="16384" width="10.83203125" style="72"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:12" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>228</v>
       </c>
@@ -18732,8 +18744,9 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="192"/>
       <c r="D3" s="1"/>
@@ -18741,8 +18754,9 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>82</v>
       </c>
@@ -18752,7 +18766,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="5"/>
     </row>
-    <row r="5" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="564" t="s">
         <v>522</v>
       </c>
@@ -18762,8 +18776,8 @@
       <c r="F5" s="565"/>
       <c r="G5" s="569"/>
     </row>
-    <row r="6" spans="2:12" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B7" s="165" t="s">
         <v>228</v>
       </c>
@@ -18776,9 +18790,10 @@
       <c r="I7" s="87"/>
       <c r="J7" s="87"/>
       <c r="K7" s="87"/>
-      <c r="L7" s="101"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L7" s="87"/>
+      <c r="M7" s="101"/>
+    </row>
+    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B8" s="166"/>
       <c r="C8" s="194"/>
       <c r="D8" s="89"/>
@@ -18789,9 +18804,10 @@
       <c r="I8" s="89"/>
       <c r="J8" s="89"/>
       <c r="K8" s="89"/>
-      <c r="L8" s="102"/>
-    </row>
-    <row r="9" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="L8" s="89"/>
+      <c r="M8" s="102"/>
+    </row>
+    <row r="9" spans="2:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B9" s="167"/>
       <c r="C9" s="175"/>
       <c r="D9" s="136" t="s">
@@ -18810,19 +18826,22 @@
         <v>351</v>
       </c>
       <c r="I9" s="136" t="s">
+        <v>657</v>
+      </c>
+      <c r="J9" s="136" t="s">
         <v>350</v>
       </c>
-      <c r="J9" s="136" t="s">
+      <c r="K9" s="136" t="s">
         <v>255</v>
       </c>
-      <c r="K9" s="136" t="s">
+      <c r="L9" s="136" t="s">
         <v>256</v>
       </c>
-      <c r="L9" s="145" t="s">
+      <c r="M9" s="145" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B10" s="168"/>
       <c r="C10" s="195"/>
       <c r="D10" s="380"/>
@@ -18833,9 +18852,10 @@
       <c r="I10" s="380"/>
       <c r="J10" s="380"/>
       <c r="K10" s="380"/>
-      <c r="L10" s="381"/>
-    </row>
-    <row r="11" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="L10" s="380"/>
+      <c r="M10" s="381"/>
+    </row>
+    <row r="11" spans="2:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="186" t="s">
         <v>332</v>
       </c>
@@ -18859,7 +18879,6 @@
         <v>0</v>
       </c>
       <c r="I11" s="362">
-        <f>'Fuel aggregation'!J25</f>
         <v>0</v>
       </c>
       <c r="J11" s="362">
@@ -18870,12 +18889,16 @@
         <f>'Fuel aggregation'!L25</f>
         <v>0</v>
       </c>
-      <c r="L11" s="382">
+      <c r="L11" s="362">
         <f>'Fuel aggregation'!M25</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="M11" s="382">
+        <f>'Fuel aggregation'!N25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B12" s="169"/>
       <c r="C12" s="188"/>
       <c r="D12" s="385"/>
@@ -18886,9 +18909,10 @@
       <c r="I12" s="385"/>
       <c r="J12" s="385"/>
       <c r="K12" s="385"/>
-      <c r="L12" s="386"/>
-    </row>
-    <row r="13" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="L12" s="385"/>
+      <c r="M12" s="386"/>
+    </row>
+    <row r="13" spans="2:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B13" s="186" t="s">
         <v>482</v>
       </c>
@@ -18901,9 +18925,10 @@
       <c r="I13" s="385"/>
       <c r="J13" s="385"/>
       <c r="K13" s="385"/>
-      <c r="L13" s="386"/>
-    </row>
-    <row r="14" spans="2:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="L13" s="385"/>
+      <c r="M13" s="386"/>
+    </row>
+    <row r="14" spans="2:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="176" t="s">
         <v>259</v>
       </c>
@@ -18916,9 +18941,10 @@
       <c r="I14" s="414"/>
       <c r="J14" s="414"/>
       <c r="K14" s="414"/>
-      <c r="L14" s="421"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L14" s="414"/>
+      <c r="M14" s="421"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B15" s="176"/>
       <c r="C15" s="188"/>
       <c r="D15" s="472"/>
@@ -18929,9 +18955,10 @@
       <c r="I15" s="472"/>
       <c r="J15" s="472"/>
       <c r="K15" s="472"/>
-      <c r="L15" s="426"/>
-    </row>
-    <row r="16" spans="2:12" ht="34" x14ac:dyDescent="0.2">
+      <c r="L15" s="472"/>
+      <c r="M15" s="426"/>
+    </row>
+    <row r="16" spans="2:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B16" s="471" t="s">
         <v>506</v>
       </c>
@@ -18956,23 +18983,27 @@
         <v>0</v>
       </c>
       <c r="I16" s="414">
+        <f>'Corrected energy balance step 2'!AK89</f>
+        <v>0</v>
+      </c>
+      <c r="J16" s="414">
         <f>SUM('Corrected energy balance step 2'!AU89,'Corrected energy balance step 2'!AZ89)</f>
         <v>0</v>
       </c>
-      <c r="J16" s="414">
+      <c r="K16" s="414">
         <f>'Corrected energy balance step 2'!BM89</f>
         <v>0</v>
       </c>
-      <c r="K16" s="406">
+      <c r="L16" s="406">
         <f>'Corrected energy balance step 2'!BK83</f>
         <v>0</v>
       </c>
-      <c r="L16" s="416">
+      <c r="M16" s="416">
         <f>SUM('Corrected energy balance step 2'!O89,'Corrected energy balance step 2'!U89,'Corrected energy balance step 2'!AT89,'Corrected energy balance step 2'!AW89:AY89,'Corrected energy balance step 2'!BA89,'Corrected energy balance step 2'!BB89:BK89)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="151"/>
       <c r="B17" s="170"/>
       <c r="C17" s="191"/>
@@ -18984,9 +19015,10 @@
       <c r="I17" s="383"/>
       <c r="J17" s="383"/>
       <c r="K17" s="383"/>
-      <c r="L17" s="384"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="L17" s="383"/>
+      <c r="M17" s="384"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B18" s="169"/>
       <c r="C18" s="188"/>
       <c r="D18" s="385"/>
@@ -18997,9 +19029,10 @@
       <c r="I18" s="385"/>
       <c r="J18" s="385"/>
       <c r="K18" s="385"/>
-      <c r="L18" s="386"/>
-    </row>
-    <row r="19" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="L18" s="385"/>
+      <c r="M18" s="386"/>
+    </row>
+    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="169" t="s">
         <v>324</v>
       </c>
@@ -19015,7 +19048,7 @@
         <v>263</v>
       </c>
       <c r="G19" s="359">
-        <f t="shared" ref="G19:L19" si="0">G11-G14-G16</f>
+        <f t="shared" ref="G19:M19" si="0">G11-G14-G16</f>
         <v>0</v>
       </c>
       <c r="H19" s="359">
@@ -19023,7 +19056,7 @@
         <v>0</v>
       </c>
       <c r="I19" s="359">
-        <f t="shared" si="0"/>
+        <f>I11-I14-I16</f>
         <v>0</v>
       </c>
       <c r="J19" s="359">
@@ -19034,12 +19067,16 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L19" s="360">
+      <c r="L19" s="359">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="M19" s="360">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="171"/>
       <c r="C20" s="190"/>
       <c r="D20" s="390"/>
@@ -19050,13 +19087,14 @@
       <c r="I20" s="390"/>
       <c r="J20" s="390"/>
       <c r="K20" s="390"/>
-      <c r="L20" s="391"/>
+      <c r="L20" s="390"/>
+      <c r="M20" s="391"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B5:G5"/>
   </mergeCells>
-  <conditionalFormatting sqref="D20:L20">
+  <conditionalFormatting sqref="D20:M20">
     <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -19064,7 +19102,7 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <ignoredErrors>
-    <ignoredError sqref="D17:L18 E19:F19" emptyCellReference="1"/>
+    <ignoredError sqref="J17:M18 E19:F19 D17:H18" emptyCellReference="1"/>
   </ignoredErrors>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -19079,10 +19117,10 @@
   <sheetPr codeName="Sheet2">
     <tabColor theme="2"/>
   </sheetPr>
-  <dimension ref="B2:D65"/>
+  <dimension ref="B2:D66"/>
   <sheetViews>
     <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+      <selection activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19753,15 +19791,26 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B64" s="149"/>
-      <c r="C64" s="147"/>
-      <c r="D64" s="148"/>
+    <row r="64" spans="2:4" ht="51" x14ac:dyDescent="0.2">
+      <c r="B64" s="149" t="s">
+        <v>658</v>
+      </c>
+      <c r="C64" s="150" t="s">
+        <v>659</v>
+      </c>
+      <c r="D64" s="148">
+        <v>1.56</v>
+      </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B65" s="16"/>
-      <c r="C65" s="9"/>
-      <c r="D65" s="244"/>
+      <c r="B65" s="149"/>
+      <c r="C65" s="147"/>
+      <c r="D65" s="148"/>
+    </row>
+    <row r="66" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B66" s="16"/>
+      <c r="C66" s="9"/>
+      <c r="D66" s="244"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -19984,10 +20033,10 @@
   <sheetPr codeName="Sheet21">
     <tabColor theme="8" tint="0.79998168889431442"/>
   </sheetPr>
-  <dimension ref="B2:M26"/>
+  <dimension ref="B2:N26"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19995,11 +20044,11 @@
     <col min="1" max="1" width="10.83203125" style="72"/>
     <col min="2" max="3" width="30.5" style="72" customWidth="1"/>
     <col min="4" max="4" width="2.83203125" style="72" customWidth="1"/>
-    <col min="5" max="13" width="15.83203125" style="72" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="72"/>
+    <col min="5" max="14" width="15.83203125" style="72" customWidth="1"/>
+    <col min="15" max="16384" width="10.83203125" style="72"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" ht="21" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>201</v>
       </c>
@@ -20010,8 +20059,9 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -20020,8 +20070,9 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
         <v>82</v>
       </c>
@@ -20032,7 +20083,7 @@
       <c r="G4" s="4"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="2:13" ht="90" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:14" ht="90" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="573" t="s">
         <v>502</v>
       </c>
@@ -20043,8 +20094,8 @@
       <c r="G5" s="574"/>
       <c r="H5" s="575"/>
     </row>
-    <row r="6" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B7" s="23" t="s">
         <v>222</v>
       </c>
@@ -20058,9 +20109,10 @@
       <c r="J7" s="42"/>
       <c r="K7" s="42"/>
       <c r="L7" s="42"/>
-      <c r="M7" s="144"/>
-    </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M7" s="42"/>
+      <c r="N7" s="144"/>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B8" s="26"/>
       <c r="C8" s="1"/>
       <c r="D8" s="7"/>
@@ -20072,9 +20124,10 @@
       <c r="J8" s="134"/>
       <c r="K8" s="134"/>
       <c r="L8" s="134"/>
-      <c r="M8" s="135"/>
-    </row>
-    <row r="9" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="M8" s="134"/>
+      <c r="N8" s="135"/>
+    </row>
+    <row r="9" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B9" s="218" t="s">
         <v>388</v>
       </c>
@@ -20096,19 +20149,22 @@
         <v>351</v>
       </c>
       <c r="J9" s="136" t="s">
+        <v>656</v>
+      </c>
+      <c r="K9" s="136" t="s">
         <v>350</v>
       </c>
-      <c r="K9" s="136" t="s">
+      <c r="L9" s="136" t="s">
         <v>255</v>
       </c>
-      <c r="L9" s="136" t="s">
+      <c r="M9" s="136" t="s">
         <v>256</v>
       </c>
-      <c r="M9" s="145" t="s">
+      <c r="N9" s="145" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B10" s="219" t="s">
         <v>206</v>
       </c>
@@ -20122,9 +20178,10 @@
       <c r="J10" s="380"/>
       <c r="K10" s="380"/>
       <c r="L10" s="380"/>
-      <c r="M10" s="381"/>
-    </row>
-    <row r="11" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="M10" s="380"/>
+      <c r="N10" s="381"/>
+    </row>
+    <row r="11" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="220"/>
       <c r="C11" s="375" t="s">
         <v>124</v>
@@ -20150,24 +20207,27 @@
         <f>SUM('Corrected energy balance step 2'!U28:AQ28)</f>
         <v>0</v>
       </c>
-      <c r="J11" s="362">
+      <c r="J11" s="362" t="s">
+        <v>263</v>
+      </c>
+      <c r="K11" s="362">
         <f>SUM('Corrected energy balance step 2'!AU28,'Corrected energy balance step 2'!AZ28)</f>
         <v>0</v>
       </c>
-      <c r="K11" s="362">
+      <c r="L11" s="362">
         <f>'Corrected energy balance step 2'!BM28</f>
         <v>0</v>
       </c>
-      <c r="L11" s="362">
+      <c r="M11" s="362">
         <f>'Corrected energy balance step 2'!BL28</f>
         <v>0</v>
       </c>
-      <c r="M11" s="382">
+      <c r="N11" s="382">
         <f>SUM('Corrected energy balance step 2'!O28,'Corrected energy balance step 2'!U28,'Corrected energy balance step 2'!AT28,'Corrected energy balance step 2'!AW28:AY28,'Corrected energy balance step 2'!BA28,'Corrected energy balance step 2'!BB28:BK28)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="220"/>
       <c r="C12" s="375" t="s">
         <v>125</v>
@@ -20193,24 +20253,27 @@
         <f>SUM('Corrected energy balance step 2'!U30:AQ30)</f>
         <v>0</v>
       </c>
-      <c r="J12" s="362">
+      <c r="J12" s="362" t="s">
+        <v>263</v>
+      </c>
+      <c r="K12" s="362">
         <f>SUM('Corrected energy balance step 2'!AU30,'Corrected energy balance step 2'!AZ30)</f>
         <v>0</v>
       </c>
-      <c r="K12" s="362">
+      <c r="L12" s="362">
         <f>'Corrected energy balance step 2'!BM30</f>
         <v>0</v>
       </c>
-      <c r="L12" s="362">
+      <c r="M12" s="362">
         <f>'Corrected energy balance step 2'!BL30</f>
         <v>0</v>
       </c>
-      <c r="M12" s="382">
+      <c r="N12" s="382">
         <f>SUM('Corrected energy balance step 2'!O30,'Corrected energy balance step 2'!U30,'Corrected energy balance step 2'!AT30,'Corrected energy balance step 2'!AW30:AY30,'Corrected energy balance step 2'!BA30,'Corrected energy balance step 2'!BB30:BK30)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13" s="377"/>
       <c r="C13" s="378"/>
       <c r="D13" s="379"/>
@@ -20222,9 +20285,10 @@
       <c r="J13" s="383"/>
       <c r="K13" s="383"/>
       <c r="L13" s="383"/>
-      <c r="M13" s="384"/>
-    </row>
-    <row r="14" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="M13" s="383"/>
+      <c r="N13" s="384"/>
+    </row>
+    <row r="14" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B14" s="221" t="s">
         <v>130</v>
       </c>
@@ -20238,9 +20302,10 @@
       <c r="J14" s="385"/>
       <c r="K14" s="385"/>
       <c r="L14" s="385"/>
-      <c r="M14" s="386"/>
-    </row>
-    <row r="15" spans="2:13" ht="51" x14ac:dyDescent="0.2">
+      <c r="M14" s="385"/>
+      <c r="N14" s="386"/>
+    </row>
+    <row r="15" spans="2:14" ht="51" x14ac:dyDescent="0.2">
       <c r="B15" s="220"/>
       <c r="C15" s="392" t="s">
         <v>501</v>
@@ -20266,24 +20331,27 @@
         <f>SUM('Corrected energy balance step 2'!V40:AQ40)+SUM('Corrected energy balance step 2'!AW40:AZ40)-SUM('Corrected energy balance step 2'!V49:AQ49)-SUM('Corrected energy balance step 2'!AW49:AZ49)-SUM('Corrected energy balance step 2'!V53:AQ53)-SUM('Corrected energy balance step 2'!AW53:AZ53)</f>
         <v>0</v>
       </c>
-      <c r="J15" s="362">
+      <c r="J15" s="362" t="s">
+        <v>263</v>
+      </c>
+      <c r="K15" s="362">
         <f>SUM('Corrected energy balance step 2'!AU40,'Corrected energy balance step 2'!AZ40)-SUM('Corrected energy balance step 2'!AU53,'Corrected energy balance step 2'!AZ53)-SUM('Corrected energy balance step 2'!AU49,'Corrected energy balance step 2'!AZ49)</f>
         <v>0</v>
       </c>
-      <c r="K15" s="362">
+      <c r="L15" s="362">
         <f>'Corrected energy balance step 2'!BM40-'Corrected energy balance step 2'!BM53-'Corrected energy balance step 2'!BM49</f>
         <v>0</v>
       </c>
-      <c r="L15" s="362">
+      <c r="M15" s="362">
         <f>'Corrected energy balance step 2'!BL40-'Corrected energy balance step 2'!BL53-'Corrected energy balance step 2'!BL49</f>
         <v>0</v>
       </c>
-      <c r="M15" s="382">
+      <c r="N15" s="382">
         <f>SUM('Corrected energy balance step 2'!O40,'Corrected energy balance step 2'!U40,'Corrected energy balance step 2'!AT40,'Corrected energy balance step 2'!AW40:AY40,'Corrected energy balance step 2'!BA40,'Corrected energy balance step 2'!BB40:BK40)-SUM('Corrected energy balance step 2'!O53,'Corrected energy balance step 2'!U53,'Corrected energy balance step 2'!AT53,'Corrected energy balance step 2'!AW53:AY53,'Corrected energy balance step 2'!BA53,'Corrected energy balance step 2'!BB53:BK53)-SUM('Corrected energy balance step 2'!O49,'Corrected energy balance step 2'!U49,'Corrected energy balance step 2'!AT49,'Corrected energy balance step 2'!AW49:AY49,'Corrected energy balance step 2'!BA49,'Corrected energy balance step 2'!BB49:BK49)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="222"/>
       <c r="C16" s="393" t="s">
         <v>124</v>
@@ -20309,24 +20377,27 @@
         <f>SUM('Corrected energy balance step 2'!U43:AQ43)+SUM('Corrected energy balance step 2'!AW43:AZ43)</f>
         <v>0</v>
       </c>
-      <c r="J16" s="362">
+      <c r="J16" s="362" t="s">
+        <v>263</v>
+      </c>
+      <c r="K16" s="362">
         <f>SUM('Corrected energy balance step 2'!AU43,'Corrected energy balance step 2'!AZ43)</f>
         <v>0</v>
       </c>
-      <c r="K16" s="362">
+      <c r="L16" s="362">
         <f>'Corrected energy balance step 2'!BM43</f>
         <v>0</v>
       </c>
-      <c r="L16" s="362">
+      <c r="M16" s="362">
         <f>'Corrected energy balance step 2'!BL43</f>
         <v>0</v>
       </c>
-      <c r="M16" s="382">
+      <c r="N16" s="382">
         <f>SUM('Corrected energy balance step 2'!O43,'Corrected energy balance step 2'!U43,'Corrected energy balance step 2'!AT43,'Corrected energy balance step 2'!AW43:AY43,'Corrected energy balance step 2'!BA43,'Corrected energy balance step 2'!BB43:BK43)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B17" s="222"/>
       <c r="C17" s="393" t="s">
         <v>125</v>
@@ -20352,24 +20423,27 @@
         <f>SUM('Corrected energy balance step 2'!U46:AQ46)+SUM('Corrected energy balance step 2'!AW46:AZ46)</f>
         <v>0</v>
       </c>
-      <c r="J17" s="362">
+      <c r="J17" s="362" t="s">
+        <v>263</v>
+      </c>
+      <c r="K17" s="362">
         <f>SUM('Corrected energy balance step 2'!AU46,'Corrected energy balance step 2'!AZ46)</f>
         <v>0</v>
       </c>
-      <c r="K17" s="362">
+      <c r="L17" s="362">
         <f>'Corrected energy balance step 2'!BM46</f>
         <v>0</v>
       </c>
-      <c r="L17" s="362">
+      <c r="M17" s="362">
         <f>'Corrected energy balance step 2'!BL46</f>
         <v>0</v>
       </c>
-      <c r="M17" s="382">
+      <c r="N17" s="382">
         <f>SUM('Corrected energy balance step 2'!O46,'Corrected energy balance step 2'!U46,'Corrected energy balance step 2'!AT46,'Corrected energy balance step 2'!AW46:AY46,'Corrected energy balance step 2'!BA46,'Corrected energy balance step 2'!BB46:BK46)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" s="377"/>
       <c r="C18" s="378"/>
       <c r="D18" s="379"/>
@@ -20381,9 +20455,10 @@
       <c r="J18" s="383"/>
       <c r="K18" s="383"/>
       <c r="L18" s="383"/>
-      <c r="M18" s="384"/>
-    </row>
-    <row r="19" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="M18" s="383"/>
+      <c r="N18" s="384"/>
+    </row>
+    <row r="19" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" s="221" t="s">
         <v>140</v>
       </c>
@@ -20397,9 +20472,10 @@
       <c r="J19" s="385"/>
       <c r="K19" s="385"/>
       <c r="L19" s="385"/>
-      <c r="M19" s="386"/>
-    </row>
-    <row r="20" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="M19" s="385"/>
+      <c r="N19" s="386"/>
+    </row>
+    <row r="20" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" s="220"/>
       <c r="C20" s="392" t="s">
         <v>24</v>
@@ -20422,27 +20498,31 @@
         <v>0</v>
       </c>
       <c r="I20" s="337">
-        <f>SUM('Corrected energy balance step 2'!U60:AQ60) + MAX(SUM('Corrected energy balance step 2'!AX60:AX60),0) + MAX(SUM('Corrected energy balance step 2'!AW60:AW60) + SUM('Corrected energy balance step 2'!AY60:AZ60),0)</f>
+        <f>SUM('Corrected energy balance step 2'!U60:AQ60) + MAX(SUM('Corrected energy balance step 2'!AX60:AX60),0) + MAX(SUM('Corrected energy balance step 2'!AW60:AW60) + SUM('Corrected energy balance step 2'!AY60:AZ60),0)-J20</f>
         <v>0</v>
       </c>
       <c r="J20" s="337">
+        <f>'Corrected energy balance step 2'!AK60</f>
+        <v>0</v>
+      </c>
+      <c r="K20" s="337">
         <f>SUM('Corrected energy balance step 2'!AU60,'Corrected energy balance step 2'!AZ60)</f>
         <v>0</v>
       </c>
-      <c r="K20" s="337">
+      <c r="L20" s="337">
         <f>'Corrected energy balance step 2'!BM60</f>
         <v>0</v>
       </c>
-      <c r="L20" s="337">
+      <c r="M20" s="337">
         <f>'Corrected energy balance step 2'!BL60</f>
         <v>0</v>
       </c>
-      <c r="M20" s="389">
+      <c r="N20" s="389">
         <f>SUM('Corrected energy balance step 2'!O60,'Corrected energy balance step 2'!U60,'Corrected energy balance step 2'!AT60,'Corrected energy balance step 2'!AW60:AY60,'Corrected energy balance step 2'!BA60,'Corrected energy balance step 2'!BB60:BK60)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B21" s="222"/>
       <c r="C21" s="393" t="s">
         <v>141</v>
@@ -20468,24 +20548,27 @@
         <f>SUM('Corrected energy balance step 2'!U61:AQ61) + MAX(SUM('Corrected energy balance step 2'!AX61:AX61),0) + MAX(SUM('Corrected energy balance step 2'!AW61:AW61) + SUM('Corrected energy balance step 2'!AY61:AZ61),0)</f>
         <v>0</v>
       </c>
-      <c r="J21" s="337">
+      <c r="J21" s="337" t="s">
+        <v>263</v>
+      </c>
+      <c r="K21" s="337">
         <f>SUM('Corrected energy balance step 2'!AU61,'Corrected energy balance step 2'!AZ61)</f>
         <v>0</v>
       </c>
-      <c r="K21" s="337">
+      <c r="L21" s="337">
         <f>'Corrected energy balance step 2'!BM61</f>
         <v>0</v>
       </c>
-      <c r="L21" s="337">
+      <c r="M21" s="337">
         <f>'Corrected energy balance step 2'!BL61</f>
         <v>0</v>
       </c>
-      <c r="M21" s="389">
+      <c r="N21" s="389">
         <f>SUM('Corrected energy balance step 2'!O61,'Corrected energy balance step 2'!U61,'Corrected energy balance step 2'!AT61,'Corrected energy balance step 2'!AW61:AY61,'Corrected energy balance step 2'!BA61,'Corrected energy balance step 2'!BB61:BK61)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B22" s="222"/>
       <c r="C22" s="393" t="s">
         <v>143</v>
@@ -20511,24 +20594,27 @@
         <f>SUM('Corrected energy balance step 2'!U63:AQ63) + MAX(SUM('Corrected energy balance step 2'!AX63:AX63),0) + MAX(SUM('Corrected energy balance step 2'!AW63:AW63) + SUM('Corrected energy balance step 2'!AY63:AZ63),0)</f>
         <v>0</v>
       </c>
-      <c r="J22" s="337">
+      <c r="J22" s="337" t="s">
+        <v>263</v>
+      </c>
+      <c r="K22" s="337">
         <f>SUM('Corrected energy balance step 2'!AU63,'Corrected energy balance step 2'!AZ63)</f>
         <v>0</v>
       </c>
-      <c r="K22" s="337">
+      <c r="L22" s="337">
         <f>'Corrected energy balance step 2'!BM63</f>
         <v>0</v>
       </c>
-      <c r="L22" s="337">
+      <c r="M22" s="337">
         <f>'Corrected energy balance step 2'!BL63</f>
         <v>0</v>
       </c>
-      <c r="M22" s="389">
+      <c r="N22" s="389">
         <f>SUM('Corrected energy balance step 2'!O63,'Corrected energy balance step 2'!U63,'Corrected energy balance step 2'!AT63,'Corrected energy balance step 2'!AW63:AY63,'Corrected energy balance step 2'!BA63,'Corrected energy balance step 2'!BB63:BK63)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B23" s="377"/>
       <c r="C23" s="378"/>
       <c r="D23" s="379"/>
@@ -20540,9 +20626,10 @@
       <c r="J23" s="383"/>
       <c r="K23" s="383"/>
       <c r="L23" s="383"/>
-      <c r="M23" s="384"/>
-    </row>
-    <row r="24" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="M23" s="383"/>
+      <c r="N23" s="384"/>
+    </row>
+    <row r="24" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="221" t="s">
         <v>166</v>
       </c>
@@ -20556,9 +20643,10 @@
       <c r="J24" s="385"/>
       <c r="K24" s="385"/>
       <c r="L24" s="385"/>
-      <c r="M24" s="386"/>
-    </row>
-    <row r="25" spans="2:13" ht="17" x14ac:dyDescent="0.2">
+      <c r="M24" s="385"/>
+      <c r="N24" s="386"/>
+    </row>
+    <row r="25" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B25" s="220"/>
       <c r="C25" s="392" t="s">
         <v>243</v>
@@ -20584,24 +20672,27 @@
         <f>SUM('Corrected energy balance step 2'!U88:AQ88)</f>
         <v>0</v>
       </c>
-      <c r="J25" s="362">
+      <c r="J25" s="362" t="s">
+        <v>263</v>
+      </c>
+      <c r="K25" s="362">
         <f>SUM('Corrected energy balance step 2'!AU88,'Corrected energy balance step 2'!AZ88)</f>
         <v>0</v>
       </c>
-      <c r="K25" s="362">
+      <c r="L25" s="362">
         <f>'Corrected energy balance step 2'!BM88</f>
         <v>0</v>
       </c>
-      <c r="L25" s="362">
+      <c r="M25" s="362">
         <f>'Corrected energy balance step 2'!BL88</f>
         <v>0</v>
       </c>
-      <c r="M25" s="382">
+      <c r="N25" s="382">
         <f>SUM('Corrected energy balance step 2'!O88,'Corrected energy balance step 2'!U88,'Corrected energy balance step 2'!AT88,'Corrected energy balance step 2'!AW88:AY88,'Corrected energy balance step 2'!BA88,'Corrected energy balance step 2'!BB88:BK88)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B26" s="75"/>
       <c r="C26" s="76"/>
       <c r="D26" s="228"/>
@@ -20613,7 +20704,8 @@
       <c r="J26" s="390"/>
       <c r="K26" s="390"/>
       <c r="L26" s="390"/>
-      <c r="M26" s="391"/>
+      <c r="M26" s="390"/>
+      <c r="N26" s="391"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -28830,8 +28922,8 @@
   </sheetPr>
   <dimension ref="B2:P77"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelRow="1" x14ac:dyDescent="0.2"/>
@@ -29904,7 +29996,7 @@
         <v>241</v>
       </c>
       <c r="E50" s="321">
-        <f>'Non-energetic cons analysis'!I19</f>
+        <f>'Non-energetic cons analysis'!J19</f>
         <v>0</v>
       </c>
       <c r="F50" s="216"/>
@@ -29934,7 +30026,7 @@
         <v>241</v>
       </c>
       <c r="E51" s="321">
-        <f>'Non-energetic cons analysis'!J19</f>
+        <f>'Non-energetic cons analysis'!K19</f>
         <v>0</v>
       </c>
       <c r="F51" s="216"/>
@@ -29964,7 +30056,7 @@
         <v>241</v>
       </c>
       <c r="E52" s="321">
-        <f>'Non-energetic cons analysis'!K19</f>
+        <f>'Non-energetic cons analysis'!L19</f>
         <v>0</v>
       </c>
       <c r="F52" s="216"/>
@@ -30437,7 +30529,7 @@
         <v>241</v>
       </c>
       <c r="E76" s="491">
-        <f>'Non-energetic cons analysis'!L19</f>
+        <f>'Non-energetic cons analysis'!M19</f>
         <v>0</v>
       </c>
       <c r="F76" s="492"/>
@@ -30449,7 +30541,7 @@
         <v>495</v>
       </c>
       <c r="L76" s="489" t="e">
-        <f>'Non-energetic cons analysis'!L19/SUM('Non-energetic cons analysis'!D19:L19)</f>
+        <f>'Non-energetic cons analysis'!M19/SUM('Non-energetic cons analysis'!D19:M19)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="M76" s="205"/>
@@ -30665,7 +30757,7 @@
   <dimension ref="B2:BO101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="W8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
       <selection pane="bottomRight" activeCell="K7" sqref="K7"/>

</xml_diff>